<commit_message>
String Repeat & Variables program edited
</commit_message>
<xml_diff>
--- a/python_syllabus.xlsx
+++ b/python_syllabus.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="85">
   <si>
     <t>Topic</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>variables.py</t>
+  </si>
+  <si>
+    <t>datatypes.py</t>
   </si>
   <si>
     <t>Strings</t>
@@ -273,12 +276,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,6 +328,65 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -332,60 +394,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -400,13 +434,20 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -417,7 +458,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -430,53 +471,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -503,37 +499,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -545,139 +649,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -706,15 +696,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -726,35 +707,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -774,17 +726,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -803,151 +758,186 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1296,7 +1286,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B65"/>
+  <dimension ref="A1:B66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1349,15 +1339,15 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="2"/>
+      <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3" t="s">
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="2"/>
       <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
@@ -1381,15 +1371,15 @@
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="2"/>
+      <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="3" t="s">
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="2"/>
       <c r="B13" s="3" t="s">
         <v>16</v>
       </c>
@@ -1431,15 +1421,15 @@
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="2"/>
+      <c r="B20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="3" t="s">
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="2"/>
       <c r="B21" s="3" t="s">
         <v>25</v>
       </c>
@@ -1451,23 +1441,23 @@
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="3" t="s">
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="2"/>
       <c r="B25" s="3" t="s">
         <v>31</v>
       </c>
@@ -1479,15 +1469,15 @@
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="2"/>
+      <c r="B27" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="3" t="s">
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="2"/>
       <c r="B28" s="3" t="s">
         <v>35</v>
       </c>
@@ -1523,15 +1513,15 @@
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="2"/>
+      <c r="B34" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="3" t="s">
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="4"/>
       <c r="B35" s="3" t="s">
         <v>43</v>
       </c>
@@ -1543,16 +1533,16 @@
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="4"/>
+      <c r="B37" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B37" s="3" t="s">
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="4"/>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="3" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1575,23 +1565,23 @@
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="4"/>
+      <c r="B42" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B43" s="5" t="s">
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="4"/>
       <c r="B44" s="5" t="s">
         <v>55</v>
       </c>
@@ -1609,31 +1599,31 @@
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="4"/>
+      <c r="B47" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B48" s="5" t="s">
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="4" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="6" t="s">
+      <c r="B49" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B49" s="7" t="s">
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="6" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="6"/>
       <c r="B50" s="7" t="s">
         <v>64</v>
       </c>
@@ -1646,13 +1636,13 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="6"/>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="7" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="6"/>
-      <c r="B53" s="7" t="s">
+      <c r="B53" s="5" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1669,43 +1659,41 @@
       </c>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="8" t="s">
+      <c r="A56" s="6"/>
+      <c r="B56" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B57" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B58" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B58" s="7" t="s">
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="8" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="4" t="s">
+      <c r="B59" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1713,7 +1701,7 @@
         <v>79</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1721,7 +1709,7 @@
         <v>80</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1729,7 +1717,7 @@
         <v>81</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1737,7 +1725,7 @@
         <v>82</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1745,21 +1733,29 @@
         <v>83</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A12:A19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="A49:A55"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A13:A20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A28:A34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="A50:A56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>

</xml_diff>

<commit_message>
Code refining in strings programs
</commit_message>
<xml_diff>
--- a/python_syllabus.xlsx
+++ b/python_syllabus.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\pythontraining\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C67CEE-EA1F-4C3A-A60D-B4282DA37F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7070"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Syllabus" sheetId="1" r:id="rId1"/>
@@ -274,14 +280,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="25">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -327,152 +327,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -481,7 +337,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -491,188 +347,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -695,253 +371,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -958,71 +392,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1280,22 +676,20 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="33.1818181818182" customWidth="1"/>
-    <col min="2" max="2" width="26.8181818181818" customWidth="1"/>
+    <col min="1" max="1" width="33.1796875" customWidth="1"/>
+    <col min="2" max="2" width="26.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1307,7 +701,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1315,37 +709,37 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="2"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="2"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="2"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="2"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="2"/>
+      <c r="A7" s="8"/>
       <c r="B7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1353,31 +747,31 @@
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="2"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="2"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="2"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="2"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1385,49 +779,49 @@
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="2"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="2"/>
+      <c r="A15" s="8"/>
       <c r="B15" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="2"/>
+      <c r="A16" s="8"/>
       <c r="B16" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="2"/>
+      <c r="A17" s="8"/>
       <c r="B17" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="2"/>
+      <c r="A18" s="8"/>
       <c r="B18" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="2"/>
+      <c r="A19" s="8"/>
       <c r="B19" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="2"/>
+      <c r="A20" s="8"/>
       <c r="B20" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -1435,13 +829,13 @@
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="2"/>
+      <c r="A22" s="8"/>
       <c r="B22" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="2"/>
+      <c r="A23" s="8"/>
       <c r="B23" s="3" t="s">
         <v>27</v>
       </c>
@@ -1455,7 +849,7 @@
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -1463,19 +857,19 @@
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="2"/>
+      <c r="A26" s="8"/>
       <c r="B26" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="2"/>
+      <c r="A27" s="8"/>
       <c r="B27" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B28" s="3" t="s">
@@ -1483,43 +877,43 @@
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="2"/>
+      <c r="A29" s="8"/>
       <c r="B29" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="2"/>
+      <c r="A30" s="8"/>
       <c r="B30" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="2"/>
+      <c r="A31" s="8"/>
       <c r="B31" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="2"/>
+      <c r="A32" s="8"/>
       <c r="B32" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="2"/>
+      <c r="A33" s="8"/>
       <c r="B33" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="2"/>
+      <c r="A34" s="8"/>
       <c r="B34" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -1527,19 +921,19 @@
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="4"/>
+      <c r="A36" s="9"/>
       <c r="B36" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="4"/>
+      <c r="A37" s="9"/>
       <c r="B37" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="9" t="s">
         <v>46</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -1547,25 +941,25 @@
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="4"/>
+      <c r="A39" s="9"/>
       <c r="B39" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="4"/>
+      <c r="A40" s="9"/>
       <c r="B40" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="4"/>
+      <c r="A41" s="9"/>
       <c r="B41" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="4"/>
+      <c r="A42" s="9"/>
       <c r="B42" s="5" t="s">
         <v>51</v>
       </c>
@@ -1579,7 +973,7 @@
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B44" s="5" t="s">
@@ -1587,19 +981,19 @@
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="4"/>
+      <c r="A45" s="9"/>
       <c r="B45" s="5" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="4"/>
+      <c r="A46" s="9"/>
       <c r="B46" s="5" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="4"/>
+      <c r="A47" s="9"/>
       <c r="B47" s="5" t="s">
         <v>58</v>
       </c>
@@ -1621,70 +1015,70 @@
       </c>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50" s="6" t="s">
+      <c r="A50" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="6" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:2">
-      <c r="A51" s="6"/>
-      <c r="B51" s="7" t="s">
+      <c r="A51" s="10"/>
+      <c r="B51" s="6" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" s="6"/>
-      <c r="B52" s="7" t="s">
+      <c r="A52" s="10"/>
+      <c r="B52" s="6" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="6"/>
+      <c r="A53" s="10"/>
       <c r="B53" s="5" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="6"/>
-      <c r="B54" s="7" t="s">
+      <c r="A54" s="10"/>
+      <c r="B54" s="6" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="6"/>
-      <c r="B55" s="7" t="s">
+      <c r="A55" s="10"/>
+      <c r="B55" s="6" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="6"/>
-      <c r="B56" s="7" t="s">
+      <c r="A56" s="10"/>
+      <c r="B56" s="6" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="57" spans="1:2">
-      <c r="A57" s="8" t="s">
+      <c r="A57" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B57" s="6" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="58" spans="1:2">
-      <c r="A58" s="8" t="s">
+      <c r="A58" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B58" s="6" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="8" t="s">
+      <c r="A59" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B59" s="6" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1746,19 +1140,18 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A28:A34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="A50:A56"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="A13:A20"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A28:A34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A38:A42"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="A50:A56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Dict and tuples modified
</commit_message>
<xml_diff>
--- a/python_syllabus.xlsx
+++ b/python_syllabus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\pythontraining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B484A1EF-C8E1-4B9B-A2BB-59416E0CE311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6A5DC3-C0DE-4D9F-8404-01AC56012A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="91">
   <si>
     <t>Topic</t>
   </si>
@@ -278,6 +278,21 @@
   </si>
   <si>
     <t>sort_vs_sorted.py</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>boolean_basics.py</t>
+  </si>
+  <si>
+    <t>types.py</t>
+  </si>
+  <si>
+    <t>Set</t>
+  </si>
+  <si>
+    <t>set_basics.py</t>
   </si>
 </sst>
 </file>
@@ -378,18 +393,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -407,9 +416,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -685,11 +702,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B67"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -710,458 +727,495 @@
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="8"/>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="8"/>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="8"/>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="8"/>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="8"/>
-      <c r="B7" t="s">
+      <c r="B7" s="11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="8"/>
+      <c r="B8" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="8"/>
-      <c r="B10" s="3" t="s">
-        <v>12</v>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="8"/>
-      <c r="B11" s="3" t="s">
-        <v>13</v>
+      <c r="B11" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="8"/>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="8"/>
+      <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="8" t="s">
+    <row r="14" spans="1:2">
+      <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="8"/>
-      <c r="B15" s="3" t="s">
-        <v>18</v>
+      <c r="B15" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="8"/>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="8"/>
+      <c r="B17" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="8"/>
-      <c r="B17" s="3" t="s">
+    <row r="18" spans="1:7">
+      <c r="A18" s="8"/>
+      <c r="B18" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="8"/>
-      <c r="B18" s="3" t="s">
+    <row r="19" spans="1:7">
+      <c r="A19" s="8"/>
+      <c r="B19" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="8"/>
-      <c r="B19" s="3" t="s">
+    <row r="20" spans="1:7">
+      <c r="A20" s="8"/>
+      <c r="B20" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="8"/>
-      <c r="B20" s="3" t="s">
+    <row r="21" spans="1:7">
+      <c r="A21" s="8"/>
+      <c r="B21" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="8"/>
-      <c r="B21" s="3" t="s">
+    <row r="22" spans="1:7">
+      <c r="A22" s="8"/>
+      <c r="B22" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="8" t="s">
+    <row r="23" spans="1:7">
+      <c r="A23" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="8"/>
-      <c r="B23" s="3" t="s">
+      <c r="D23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="8"/>
+      <c r="B24" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="8"/>
-      <c r="B24" s="3" t="s">
+      <c r="D24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="8"/>
+      <c r="B25" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="2" t="s">
+      <c r="D25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="8" t="s">
+      <c r="D26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="8"/>
-      <c r="B27" s="3" t="s">
+    <row r="30" spans="1:7">
+      <c r="A30" s="8"/>
+      <c r="B30" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="8"/>
-      <c r="B28" s="3" t="s">
+    <row r="31" spans="1:7">
+      <c r="A31" s="8"/>
+      <c r="B31" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="8" t="s">
+    <row r="32" spans="1:7">
+      <c r="A32" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="8"/>
-      <c r="B30" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="8"/>
-      <c r="B31" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="8"/>
-      <c r="B32" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="8"/>
-      <c r="B33" s="3" t="s">
-        <v>39</v>
+      <c r="B33" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="8"/>
-      <c r="B34" s="3" t="s">
-        <v>40</v>
+      <c r="B34" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="8"/>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="8"/>
+      <c r="B36" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="8"/>
+      <c r="B37" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="8"/>
+      <c r="B38" s="2" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="9"/>
-      <c r="B37" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="9"/>
-      <c r="B38" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="9"/>
-      <c r="B40" s="5" t="s">
-        <v>48</v>
+      <c r="B40" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="9"/>
-      <c r="B41" s="5" t="s">
-        <v>49</v>
+      <c r="B41" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="9"/>
-      <c r="B42" s="5" t="s">
-        <v>50</v>
+      <c r="A42" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="9"/>
-      <c r="B43" s="5" t="s">
-        <v>51</v>
+      <c r="B43" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>53</v>
+      <c r="A44" s="9"/>
+      <c r="B44" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>55</v>
+      <c r="A45" s="9"/>
+      <c r="B45" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="9"/>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="9"/>
+      <c r="B49" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="9"/>
-      <c r="B47" s="5" t="s">
+    <row r="50" spans="1:2">
+      <c r="A50" s="9"/>
+      <c r="B50" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="9"/>
-      <c r="B48" s="5" t="s">
+    <row r="51" spans="1:2">
+      <c r="A51" s="9"/>
+      <c r="B51" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="4" t="s">
+    <row r="52" spans="1:2">
+      <c r="A52" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B52" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="4" t="s">
+    <row r="53" spans="1:2">
+      <c r="A53" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B53" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="10" t="s">
+    <row r="54" spans="1:2">
+      <c r="A54" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B54" s="4" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="10"/>
-      <c r="B52" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="10"/>
-      <c r="B53" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="10"/>
-      <c r="B54" s="5" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="10"/>
-      <c r="B55" s="6" t="s">
-        <v>68</v>
+      <c r="B55" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="10"/>
-      <c r="B56" s="6" t="s">
-        <v>69</v>
+      <c r="B56" s="4" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="10"/>
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="10"/>
+      <c r="B58" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="10"/>
+      <c r="B59" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="10"/>
+      <c r="B60" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="7" t="s">
+    <row r="61" spans="1:2">
+      <c r="A61" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="B61" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="7" t="s">
+    <row r="62" spans="1:2">
+      <c r="A62" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="B62" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="7" t="s">
+    <row r="63" spans="1:2">
+      <c r="A63" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="B63" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="4" t="s">
+    <row r="64" spans="1:2">
+      <c r="A64" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B64" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="4" t="s">
+    <row r="65" spans="1:2">
+      <c r="A65" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B65" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="4" t="s">
+    <row r="66" spans="1:2">
+      <c r="A66" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B66" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="4" t="s">
+    <row r="67" spans="1:2">
+      <c r="A67" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B67" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="4" t="s">
+    <row r="68" spans="1:2">
+      <c r="A68" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B68" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="4" t="s">
+    <row r="69" spans="1:2">
+      <c r="A69" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B69" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="4" t="s">
+    <row r="70" spans="1:2">
+      <c r="A70" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B70" s="3" t="s">
         <v>78</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="A39:A43"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="A51:A57"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="A14:A22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A32:A38"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A42:A46"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="A54:A60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Dict and Set modified
</commit_message>
<xml_diff>
--- a/python_syllabus.xlsx
+++ b/python_syllabus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\pythontraining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6A5DC3-C0DE-4D9F-8404-01AC56012A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{086175C0-877F-4D2A-AA62-6DC5F1824F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="92">
   <si>
     <t>Topic</t>
   </si>
@@ -121,9 +121,6 @@
     <t>dictionary_formatting.py</t>
   </si>
   <si>
-    <t>del.py</t>
-  </si>
-  <si>
     <t>File Handling</t>
   </si>
   <si>
@@ -293,6 +290,12 @@
   </si>
   <si>
     <t>set_basics.py</t>
+  </si>
+  <si>
+    <t>dict_comprehension.py</t>
+  </si>
+  <si>
+    <t>delete.py</t>
   </si>
 </sst>
 </file>
@@ -393,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -416,17 +419,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,7 +701,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:B71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -724,7 +723,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -732,43 +731,43 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="8"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="8"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="8"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="8"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="11" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="11" t="s">
-        <v>88</v>
+      <c r="A8" s="9"/>
+      <c r="B8" s="8" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -776,31 +775,31 @@
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="8"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="8"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="8"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="8"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -808,414 +807,405 @@
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="8"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="8"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="8"/>
+    <row r="17" spans="1:2">
+      <c r="A17" s="9"/>
       <c r="B17" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="8"/>
+    <row r="18" spans="1:2">
+      <c r="A18" s="9"/>
       <c r="B18" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="8"/>
+    <row r="19" spans="1:2">
+      <c r="A19" s="9"/>
       <c r="B19" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="8"/>
+    <row r="20" spans="1:2">
+      <c r="A20" s="9"/>
       <c r="B20" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="8"/>
+    <row r="21" spans="1:2">
+      <c r="A21" s="9"/>
       <c r="B21" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="8"/>
+    <row r="22" spans="1:2">
+      <c r="A22" s="9"/>
       <c r="B22" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="8"/>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="9"/>
       <c r="B24" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="8"/>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="9"/>
       <c r="B25" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-    </row>
-    <row r="26" spans="1:7">
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-    </row>
-    <row r="27" spans="1:7">
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="6" t="s">
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="9"/>
+      <c r="B29" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="9"/>
+      <c r="B30" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="9"/>
+      <c r="B31" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="8"/>
-      <c r="B30" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="8"/>
-      <c r="B31" s="2" t="s">
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="8" t="s">
+      <c r="B33" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="2" t="s">
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="9"/>
+      <c r="B34" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="8"/>
-      <c r="B33" s="2" t="s">
+    <row r="35" spans="1:2">
+      <c r="A35" s="9"/>
+      <c r="B35" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="8"/>
-      <c r="B34" s="2" t="s">
+    <row r="36" spans="1:2">
+      <c r="A36" s="9"/>
+      <c r="B36" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="8"/>
-      <c r="B35" s="2" t="s">
+    <row r="37" spans="1:2">
+      <c r="A37" s="9"/>
+      <c r="B37" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="8"/>
-      <c r="B36" s="2" t="s">
+    <row r="38" spans="1:2">
+      <c r="A38" s="9"/>
+      <c r="B38" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="8"/>
-      <c r="B37" s="2" t="s">
+    <row r="39" spans="1:2">
+      <c r="A39" s="9"/>
+      <c r="B39" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="8"/>
-      <c r="B38" s="2" t="s">
+    <row r="40" spans="1:2">
+      <c r="A40" s="10" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="9" t="s">
+      <c r="B40" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="2" t="s">
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="10"/>
+      <c r="B41" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="9"/>
-      <c r="B40" s="2" t="s">
+    <row r="42" spans="1:2">
+      <c r="A42" s="10"/>
+      <c r="B42" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="9"/>
-      <c r="B41" s="2" t="s">
+    <row r="43" spans="1:2">
+      <c r="A43" s="10" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="9" t="s">
+      <c r="B43" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B42" s="2" t="s">
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="10"/>
+      <c r="B44" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="9"/>
-      <c r="B43" s="3" t="s">
+    <row r="45" spans="1:2">
+      <c r="A45" s="10"/>
+      <c r="B45" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="9"/>
-      <c r="B44" s="3" t="s">
+    <row r="46" spans="1:2">
+      <c r="A46" s="10"/>
+      <c r="B46" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="9"/>
-      <c r="B45" s="3" t="s">
+    <row r="47" spans="1:2">
+      <c r="A47" s="10"/>
+      <c r="B47" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="9"/>
-      <c r="B46" s="3" t="s">
+    <row r="48" spans="1:2">
+      <c r="A48" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="7" t="s">
+      <c r="B48" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="3" t="s">
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="10" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="9" t="s">
+      <c r="B49" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="3" t="s">
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="10"/>
+      <c r="B50" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="9"/>
-      <c r="B49" s="3" t="s">
+    <row r="51" spans="1:2">
+      <c r="A51" s="10"/>
+      <c r="B51" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="9"/>
-      <c r="B50" s="3" t="s">
+    <row r="52" spans="1:2">
+      <c r="A52" s="10"/>
+      <c r="B52" s="3" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="9"/>
-      <c r="B51" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B54" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B53" s="3" t="s">
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="10" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="10" t="s">
+      <c r="B55" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="10"/>
-      <c r="B55" s="4" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="10"/>
       <c r="B56" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="10"/>
-      <c r="B57" s="3" t="s">
-        <v>67</v>
+      <c r="B57" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="10"/>
-      <c r="B58" s="4" t="s">
-        <v>68</v>
+      <c r="B58" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="10"/>
       <c r="B59" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="10"/>
       <c r="B60" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="61" spans="1:2">
-      <c r="A61" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="A61" s="10"/>
       <c r="B61" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B64" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A33:A39"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="A43:A47"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="A55:A61"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="A14:A22"/>
     <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A32:A38"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="A42:A46"/>
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="A54:A60"/>
+    <mergeCell ref="A28:A31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
File handling concepts extended
</commit_message>
<xml_diff>
--- a/python_syllabus.xlsx
+++ b/python_syllabus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\pythontraining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{086175C0-877F-4D2A-AA62-6DC5F1824F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B7641D-6ED2-4D29-ACC5-7245ACD35417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="94">
   <si>
     <t>Topic</t>
   </si>
@@ -296,6 +296,12 @@
   </si>
   <si>
     <t>delete.py</t>
+  </si>
+  <si>
+    <t>file_overwrite.py</t>
+  </si>
+  <si>
+    <t>file_methods.py</t>
   </si>
 </sst>
 </file>
@@ -701,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B71"/>
+  <dimension ref="A1:B73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -947,216 +953,212 @@
     <row r="36" spans="1:2">
       <c r="A36" s="9"/>
       <c r="B36" s="2" t="s">
-        <v>37</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="9"/>
       <c r="B37" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="9"/>
       <c r="B38" s="2" t="s">
-        <v>39</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="9"/>
       <c r="B39" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="9"/>
+      <c r="B40" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="9"/>
+      <c r="B41" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="10" t="s">
+    <row r="42" spans="1:2">
+      <c r="A42" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="10"/>
-      <c r="B41" s="2" t="s">
+    <row r="43" spans="1:2">
+      <c r="A43" s="10"/>
+      <c r="B43" s="2" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="10"/>
-      <c r="B42" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="10"/>
-      <c r="B44" s="3" t="s">
-        <v>47</v>
+      <c r="B44" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="10"/>
-      <c r="B45" s="3" t="s">
-        <v>48</v>
+      <c r="A45" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="10"/>
       <c r="B46" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="10"/>
       <c r="B47" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="10"/>
+      <c r="B48" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="10"/>
+      <c r="B49" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="7" t="s">
+    <row r="50" spans="1:2">
+      <c r="A50" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B50" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="10" t="s">
+    <row r="51" spans="1:2">
+      <c r="A51" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B51" s="3" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="10"/>
-      <c r="B50" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="10"/>
-      <c r="B51" s="3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="10"/>
       <c r="B52" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="10"/>
+      <c r="B53" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="10"/>
+      <c r="B54" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="7" t="s">
+    <row r="55" spans="1:2">
+      <c r="A55" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B55" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="7" t="s">
+    <row r="56" spans="1:2">
+      <c r="A56" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B56" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="10" t="s">
+    <row r="57" spans="1:2">
+      <c r="A57" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B57" s="4" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="10"/>
-      <c r="B56" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="10"/>
-      <c r="B57" s="4" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="10"/>
-      <c r="B58" s="3" t="s">
-        <v>66</v>
+      <c r="B58" s="4" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="10"/>
       <c r="B59" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="10"/>
-      <c r="B60" s="4" t="s">
-        <v>68</v>
+      <c r="B60" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="10"/>
       <c r="B61" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="10"/>
+      <c r="B62" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="10"/>
+      <c r="B63" s="4" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B66" s="4" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>77</v>
@@ -1164,7 +1166,7 @@
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>77</v>
@@ -1172,7 +1174,7 @@
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>77</v>
@@ -1180,7 +1182,7 @@
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>77</v>
@@ -1188,24 +1190,40 @@
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>77</v>
       </c>
     </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A33:A39"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="A43:A47"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="A55:A61"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="A14:A22"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A33:A41"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A45:A49"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A57:A63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
File handling concepts modified
</commit_message>
<xml_diff>
--- a/python_syllabus.xlsx
+++ b/python_syllabus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\pythontraining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B7641D-6ED2-4D29-ACC5-7245ACD35417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3BB9253-EEC0-4CAD-A6AD-061094BAECEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -710,8 +710,8 @@
   <dimension ref="A1:B73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -1214,16 +1214,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A33:A41"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A45:A49"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A57:A63"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="A14:A22"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A33:A41"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="A45:A49"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A57:A63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Spaces removed in directory name and file handling modified
</commit_message>
<xml_diff>
--- a/python_syllabus.xlsx
+++ b/python_syllabus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\pythontraining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3BB9253-EEC0-4CAD-A6AD-061094BAECEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE02967-3F16-4468-88F9-05D8AC7CF81C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -139,9 +139,6 @@
     <t>file_unicode.py</t>
   </si>
   <si>
-    <t>input.py</t>
-  </si>
-  <si>
     <t>file_system_cmds.py</t>
   </si>
   <si>
@@ -302,6 +299,9 @@
   </si>
   <si>
     <t>file_methods.py</t>
+  </si>
+  <si>
+    <t>user_input.py</t>
   </si>
 </sst>
 </file>
@@ -710,8 +710,8 @@
   <dimension ref="A1:B73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B54" sqref="B54"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -769,461 +769,461 @@
     <row r="8" spans="1:2">
       <c r="A8" s="9"/>
       <c r="B8" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="9"/>
-      <c r="B10" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="9"/>
       <c r="B11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="9"/>
       <c r="B12" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="9"/>
       <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="9"/>
+      <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="9" t="s">
+    <row r="15" spans="1:2">
+      <c r="A15" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="9"/>
-      <c r="B15" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="9"/>
       <c r="B16" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="9"/>
       <c r="B17" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="9"/>
       <c r="B18" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="9"/>
       <c r="B19" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="9"/>
       <c r="B20" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="9"/>
       <c r="B21" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="9"/>
       <c r="B22" s="2" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="9"/>
+      <c r="B23" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="9"/>
-      <c r="B24" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="9"/>
       <c r="B25" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="9"/>
+      <c r="B26" s="2" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="9" t="s">
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="9"/>
-      <c r="B29" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="9"/>
       <c r="B30" s="2" t="s">
-        <v>90</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="9"/>
       <c r="B31" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="9"/>
+      <c r="B32" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="9" t="s">
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="9"/>
-      <c r="B34" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="9"/>
       <c r="B35" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="9"/>
       <c r="B36" s="2" t="s">
-        <v>92</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="9"/>
       <c r="B37" s="2" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="9"/>
       <c r="B38" s="2" t="s">
-        <v>93</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="9"/>
       <c r="B39" s="2" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="9"/>
       <c r="B40" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="9"/>
       <c r="B41" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="10"/>
       <c r="B43" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="10"/>
       <c r="B44" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="10"/>
       <c r="B46" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="10"/>
       <c r="B47" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="10"/>
       <c r="B48" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="10"/>
       <c r="B49" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="10"/>
       <c r="B52" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="10"/>
       <c r="B53" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="10"/>
       <c r="B54" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B57" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="10"/>
       <c r="B58" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="10"/>
       <c r="B59" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="10"/>
       <c r="B60" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="10"/>
       <c r="B61" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="10"/>
       <c r="B62" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="10"/>
       <c r="B63" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B64" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B65" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B66" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B67" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A33:A41"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A15:A23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A34:A41"/>
     <mergeCell ref="A42:A44"/>
     <mergeCell ref="A45:A49"/>
     <mergeCell ref="A51:A54"/>
     <mergeCell ref="A57:A63"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A9:A13"/>
-    <mergeCell ref="A14:A22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A28:A31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Regex match concepts modified
</commit_message>
<xml_diff>
--- a/python_syllabus.xlsx
+++ b/python_syllabus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\pythontraining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE02967-3F16-4468-88F9-05D8AC7CF81C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCD6C64-8949-4301-AC84-11EF0CA4F24A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -320,13 +320,13 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -334,7 +334,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -342,7 +342,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -351,7 +351,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -710,8 +710,8 @@
   <dimension ref="A1:B73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -1214,16 +1214,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A34:A41"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A45:A49"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A57:A63"/>
     <mergeCell ref="A2:A9"/>
     <mergeCell ref="A10:A14"/>
     <mergeCell ref="A15:A23"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A34:A41"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="A45:A49"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A57:A63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Subprocess, Modules and Packages refined
</commit_message>
<xml_diff>
--- a/python_syllabus.xlsx
+++ b/python_syllabus.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\pythontraining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1811436A-FEB1-4BBA-B8D8-C4DBE9F9A24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD733389-4A3C-44FF-9B2C-2CE31B9C76E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -256,9 +256,6 @@
     <t>Lambda Functions&amp; map/reduce/filter</t>
   </si>
   <si>
-    <t xml:space="preserve">Threads </t>
-  </si>
-  <si>
     <t>Accessing API</t>
   </si>
   <si>
@@ -302,6 +299,9 @@
   </si>
   <si>
     <t>user_input.py</t>
+  </si>
+  <si>
+    <t>Threading</t>
   </si>
 </sst>
 </file>
@@ -710,8 +710,8 @@
   <dimension ref="A1:B73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B51" sqref="B51"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -769,13 +769,13 @@
     <row r="8" spans="1:2">
       <c r="A8" s="9"/>
       <c r="B8" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="9"/>
       <c r="B9" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -863,7 +863,7 @@
     <row r="23" spans="1:2">
       <c r="A23" s="9"/>
       <c r="B23" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -896,10 +896,10 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -919,21 +919,21 @@
     <row r="31" spans="1:2">
       <c r="A31" s="9"/>
       <c r="B31" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="9"/>
       <c r="B32" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -959,7 +959,7 @@
     <row r="37" spans="1:2">
       <c r="A37" s="9"/>
       <c r="B37" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -971,7 +971,7 @@
     <row r="39" spans="1:2">
       <c r="A39" s="9"/>
       <c r="B39" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1174,7 +1174,7 @@
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>76</v>
@@ -1182,7 +1182,7 @@
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>76</v>
@@ -1190,7 +1190,7 @@
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>76</v>
@@ -1198,7 +1198,7 @@
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>76</v>
@@ -1206,7 +1206,7 @@
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>76</v>
@@ -1214,16 +1214,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A34:A41"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A45:A49"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A57:A63"/>
     <mergeCell ref="A2:A9"/>
     <mergeCell ref="A10:A14"/>
     <mergeCell ref="A15:A23"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A34:A41"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="A45:A49"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A57:A63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
oops edited and directories restructured
</commit_message>
<xml_diff>
--- a/python_syllabus.xlsx
+++ b/python_syllabus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\pythontraining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F94B857-C65D-44C2-AF7D-5ADE5297FE3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A54A7FC8-323E-428A-84F6-C43095383E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="107">
   <si>
     <t>Topic</t>
   </si>
@@ -211,39 +211,21 @@
     <t>objects.py</t>
   </si>
   <si>
-    <t>classes.py</t>
-  </si>
-  <si>
     <t>inheritance.py</t>
   </si>
   <si>
     <t>data_hiding.py</t>
   </si>
   <si>
-    <t>overriding.py</t>
-  </si>
-  <si>
-    <t>overloading.py</t>
-  </si>
-  <si>
     <t>encapsulation.py</t>
   </si>
   <si>
-    <t>Decorator</t>
-  </si>
-  <si>
     <t>decorator.py</t>
   </si>
   <si>
-    <t>Iterator</t>
-  </si>
-  <si>
     <t>iterator.py</t>
   </si>
   <si>
-    <t>Generator</t>
-  </si>
-  <si>
     <t>generator.py</t>
   </si>
   <si>
@@ -253,9 +235,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>Lambda Functions&amp; map/reduce/filter</t>
-  </si>
-  <si>
     <t>Accessing API</t>
   </si>
   <si>
@@ -302,6 +281,66 @@
   </si>
   <si>
     <t>Threading</t>
+  </si>
+  <si>
+    <t>class_oops.py</t>
+  </si>
+  <si>
+    <t>polymorphism.py (overloading | overriding)</t>
+  </si>
+  <si>
+    <t>Map / Reduce / Filter</t>
+  </si>
+  <si>
+    <t>Decorator / Iterator / Generator</t>
+  </si>
+  <si>
+    <t>counters.py</t>
+  </si>
+  <si>
+    <t>ordereddict.py</t>
+  </si>
+  <si>
+    <t>defaultdict.py</t>
+  </si>
+  <si>
+    <t>chainmap.py</t>
+  </si>
+  <si>
+    <t>namedtuple.py</t>
+  </si>
+  <si>
+    <t>deque.py</t>
+  </si>
+  <si>
+    <t>userdict.py</t>
+  </si>
+  <si>
+    <t>userlist.py</t>
+  </si>
+  <si>
+    <t>userstring.py</t>
+  </si>
+  <si>
+    <t>ordereddict_delete_insert.py</t>
+  </si>
+  <si>
+    <t>lambda_function.py</t>
+  </si>
+  <si>
+    <t>map_function.py</t>
+  </si>
+  <si>
+    <t>reduce_function.py</t>
+  </si>
+  <si>
+    <t>filter_function.py</t>
+  </si>
+  <si>
+    <t>threading.py</t>
+  </si>
+  <si>
+    <t>thread_details.py</t>
   </si>
 </sst>
 </file>
@@ -375,7 +414,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -398,11 +437,79 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -416,9 +523,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -430,6 +534,33 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -707,17 +838,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B73"/>
+  <dimension ref="A1:B85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B72" sqref="B72"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="33.1796875" customWidth="1"/>
-    <col min="2" max="2" width="26.81640625" customWidth="1"/>
+    <col min="2" max="2" width="37.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -729,7 +860,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -737,49 +868,49 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="9"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="9"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="9"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="9"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="9"/>
-      <c r="B7" s="8" t="s">
+      <c r="A7" s="8"/>
+      <c r="B7" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="9"/>
-      <c r="B8" s="8" t="s">
+      <c r="A8" s="8"/>
+      <c r="B8" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="8"/>
+      <c r="B9" s="7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="9"/>
-      <c r="B9" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -787,31 +918,31 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="9"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="9"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="9"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="9"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -819,55 +950,55 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="9"/>
+      <c r="A16" s="8"/>
       <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="9"/>
+      <c r="A17" s="8"/>
       <c r="B17" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="9"/>
+      <c r="A18" s="8"/>
       <c r="B18" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="9"/>
+      <c r="A19" s="8"/>
       <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="9"/>
+      <c r="A20" s="8"/>
       <c r="B20" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="9"/>
+      <c r="A21" s="8"/>
       <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="9"/>
+      <c r="A22" s="8"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="9"/>
+      <c r="A23" s="8"/>
       <c r="B23" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -875,19 +1006,19 @@
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="9"/>
+      <c r="A25" s="8"/>
       <c r="B25" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="9"/>
+      <c r="A26" s="8"/>
       <c r="B26" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -895,15 +1026,15 @@
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="6" t="s">
-        <v>83</v>
+      <c r="A28" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -911,33 +1042,33 @@
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="9"/>
+      <c r="A30" s="8"/>
       <c r="B30" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="9"/>
+      <c r="A31" s="8"/>
       <c r="B31" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="9"/>
+      <c r="A32" s="8"/>
       <c r="B32" s="2" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="6" t="s">
-        <v>86</v>
+      <c r="A33" s="5" t="s">
+        <v>79</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="8" t="s">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -945,49 +1076,49 @@
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="9"/>
+      <c r="A35" s="8"/>
       <c r="B35" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="9"/>
+      <c r="A36" s="8"/>
       <c r="B36" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="9"/>
+      <c r="A37" s="8"/>
       <c r="B37" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="9"/>
+      <c r="A38" s="8"/>
       <c r="B38" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="9"/>
+      <c r="A39" s="8"/>
       <c r="B39" s="2" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="9"/>
+      <c r="A40" s="8"/>
       <c r="B40" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="9"/>
+      <c r="A41" s="8"/>
       <c r="B41" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="9" t="s">
         <v>40</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -995,19 +1126,19 @@
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="10"/>
+      <c r="A43" s="9"/>
       <c r="B43" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="10"/>
+      <c r="A44" s="9"/>
       <c r="B44" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="10" t="s">
+      <c r="A45" s="9" t="s">
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -1015,31 +1146,31 @@
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="10"/>
+      <c r="A46" s="9"/>
       <c r="B46" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="10"/>
+      <c r="A47" s="9"/>
       <c r="B47" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="10"/>
+      <c r="A48" s="9"/>
       <c r="B48" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="10"/>
+      <c r="A49" s="9"/>
       <c r="B49" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50" s="7" t="s">
+      <c r="A50" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B50" s="3" t="s">
@@ -1047,7 +1178,7 @@
       </c>
     </row>
     <row r="51" spans="1:2">
-      <c r="A51" s="10" t="s">
+      <c r="A51" s="9" t="s">
         <v>52</v>
       </c>
       <c r="B51" s="3" t="s">
@@ -1055,25 +1186,25 @@
       </c>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" s="10"/>
+      <c r="A52" s="9"/>
       <c r="B52" s="3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="10"/>
+      <c r="A53" s="9"/>
       <c r="B53" s="3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="10"/>
+      <c r="A54" s="9"/>
       <c r="B54" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="6" t="s">
         <v>57</v>
       </c>
       <c r="B55" s="3" t="s">
@@ -1081,7 +1212,7 @@
       </c>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="7" t="s">
+      <c r="A56" s="16" t="s">
         <v>59</v>
       </c>
       <c r="B56" s="3" t="s">
@@ -1089,141 +1220,214 @@
       </c>
     </row>
     <row r="57" spans="1:2">
-      <c r="A57" s="10" t="s">
+      <c r="A57" s="18"/>
+      <c r="B57" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B58" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="10"/>
-      <c r="B58" s="4" t="s">
+    <row r="59" spans="1:2">
+      <c r="A59" s="9"/>
+      <c r="B59" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="9"/>
+      <c r="B60" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="10"/>
-      <c r="B59" s="4" t="s">
+    <row r="61" spans="1:2">
+      <c r="A61" s="9"/>
+      <c r="B61" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="10"/>
-      <c r="B60" s="3" t="s">
+    <row r="62" spans="1:2">
+      <c r="A62" s="9"/>
+      <c r="B62" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="9"/>
+      <c r="B63" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="10"/>
-      <c r="B61" s="4" t="s">
+    <row r="64" spans="1:2">
+      <c r="A64" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B64" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="10"/>
-      <c r="B62" s="4" t="s">
+    <row r="65" spans="1:2">
+      <c r="A65" s="11"/>
+      <c r="B65" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="10"/>
-      <c r="B63" s="4" t="s">
+    <row r="66" spans="1:2">
+      <c r="A66" s="12"/>
+      <c r="B66" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="5" t="s">
+    <row r="67" spans="1:2">
+      <c r="A67" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B67" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="14"/>
+      <c r="B68" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="14"/>
+      <c r="B69" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="14"/>
+      <c r="B70" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="14"/>
+      <c r="B71" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="14"/>
+      <c r="B72" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="14"/>
+      <c r="B73" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="14"/>
+      <c r="B74" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="14"/>
+      <c r="B75" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="15"/>
+      <c r="B76" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="17"/>
+      <c r="B78" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="18"/>
+      <c r="B79" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="15"/>
+      <c r="B81" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B82" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B65" s="4" t="s">
+    <row r="83" spans="1:2">
+      <c r="A83" s="6" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="5" t="s">
+      <c r="B83" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B84" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="6" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
-      <c r="A71" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
-      <c r="A72" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>76</v>
+      <c r="B85" s="3" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="15">
+    <mergeCell ref="A64:A66"/>
+    <mergeCell ref="A67:A76"/>
+    <mergeCell ref="A77:A79"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A80:A81"/>
+    <mergeCell ref="A34:A41"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A45:A49"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A58:A63"/>
     <mergeCell ref="A2:A9"/>
     <mergeCell ref="A10:A14"/>
     <mergeCell ref="A15:A23"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A34:A41"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="A45:A49"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A57:A63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added named parameter & collections modified
</commit_message>
<xml_diff>
--- a/python_syllabus.xlsx
+++ b/python_syllabus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\pythontraining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A54A7FC8-323E-428A-84F6-C43095383E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722B7246-C709-4072-AB0B-59D1F3952241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="108">
   <si>
     <t>Topic</t>
   </si>
@@ -341,6 +341,9 @@
   </si>
   <si>
     <t>thread_details.py</t>
+  </si>
+  <si>
+    <t>named_parameters.py</t>
   </si>
 </sst>
 </file>
@@ -530,37 +533,37 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -838,11 +841,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B85"/>
+  <dimension ref="A1:B86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -860,7 +863,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -868,49 +871,49 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="8"/>
+      <c r="A3" s="17"/>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="8"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="8"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="8"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="8"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="8"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="7" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="8"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="7" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -918,31 +921,31 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="8"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="8"/>
+      <c r="A12" s="17"/>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="8"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="8"/>
+      <c r="A14" s="17"/>
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="17" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -950,55 +953,55 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="8"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="8"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="8"/>
+      <c r="A18" s="17"/>
       <c r="B18" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="8"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="8"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="8"/>
+      <c r="A21" s="17"/>
       <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="8"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="8"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="2" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="17" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1006,13 +1009,13 @@
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="8"/>
+      <c r="A25" s="17"/>
       <c r="B25" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="8"/>
+      <c r="A26" s="17"/>
       <c r="B26" s="2" t="s">
         <v>27</v>
       </c>
@@ -1034,7 +1037,7 @@
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="17" t="s">
         <v>30</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1042,19 +1045,19 @@
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="8"/>
+      <c r="A30" s="17"/>
       <c r="B30" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="8"/>
+      <c r="A31" s="17"/>
       <c r="B31" s="2" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="8"/>
+      <c r="A32" s="17"/>
       <c r="B32" s="2" t="s">
         <v>82</v>
       </c>
@@ -1068,7 +1071,7 @@
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="17" t="s">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -1076,49 +1079,49 @@
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="8"/>
+      <c r="A35" s="17"/>
       <c r="B35" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="8"/>
+      <c r="A36" s="17"/>
       <c r="B36" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="8"/>
+      <c r="A37" s="17"/>
       <c r="B37" s="2" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="8"/>
+      <c r="A38" s="17"/>
       <c r="B38" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="8"/>
+      <c r="A39" s="17"/>
       <c r="B39" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="8"/>
+      <c r="A40" s="17"/>
       <c r="B40" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="8"/>
+      <c r="A41" s="17"/>
       <c r="B41" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="18" t="s">
         <v>40</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -1126,19 +1129,19 @@
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="9"/>
+      <c r="A43" s="18"/>
       <c r="B43" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="9"/>
+      <c r="A44" s="18"/>
       <c r="B44" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="18" t="s">
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -1146,25 +1149,25 @@
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="9"/>
+      <c r="A46" s="18"/>
       <c r="B46" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="9"/>
+      <c r="A47" s="18"/>
       <c r="B47" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="9"/>
+      <c r="A48" s="18"/>
       <c r="B48" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="9"/>
+      <c r="A49" s="18"/>
       <c r="B49" s="3" t="s">
         <v>49</v>
       </c>
@@ -1178,7 +1181,7 @@
       </c>
     </row>
     <row r="51" spans="1:2">
-      <c r="A51" s="9" t="s">
+      <c r="A51" s="18" t="s">
         <v>52</v>
       </c>
       <c r="B51" s="3" t="s">
@@ -1186,19 +1189,19 @@
       </c>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" s="9"/>
+      <c r="A52" s="18"/>
       <c r="B52" s="3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="9"/>
+      <c r="A53" s="18"/>
       <c r="B53" s="3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="9"/>
+      <c r="A54" s="18"/>
       <c r="B54" s="3" t="s">
         <v>56</v>
       </c>
@@ -1212,7 +1215,7 @@
       </c>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="16" t="s">
+      <c r="A56" s="14" t="s">
         <v>59</v>
       </c>
       <c r="B56" s="3" t="s">
@@ -1220,176 +1223,174 @@
       </c>
     </row>
     <row r="57" spans="1:2">
-      <c r="A57" s="18"/>
+      <c r="A57" s="15"/>
       <c r="B57" s="3" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="58" spans="1:2">
-      <c r="A58" s="9" t="s">
+      <c r="A58" s="16"/>
+      <c r="B58" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B59" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="9"/>
-      <c r="B59" s="4" t="s">
+    <row r="60" spans="1:2">
+      <c r="A60" s="18"/>
+      <c r="B60" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="9"/>
-      <c r="B60" s="4" t="s">
+    <row r="61" spans="1:2">
+      <c r="A61" s="18"/>
+      <c r="B61" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="9"/>
-      <c r="B61" s="3" t="s">
+    <row r="62" spans="1:2">
+      <c r="A62" s="18"/>
+      <c r="B62" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="9"/>
-      <c r="B62" s="4" t="s">
+    <row r="63" spans="1:2">
+      <c r="A63" s="18"/>
+      <c r="B63" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="9"/>
-      <c r="B63" s="4" t="s">
+    <row r="64" spans="1:2">
+      <c r="A64" s="18"/>
+      <c r="B64" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="10" t="s">
+    <row r="65" spans="1:2">
+      <c r="A65" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B65" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="11"/>
-      <c r="B65" s="4" t="s">
+    <row r="66" spans="1:2">
+      <c r="A66" s="9"/>
+      <c r="B66" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="12"/>
-      <c r="B66" s="4" t="s">
+    <row r="67" spans="1:2">
+      <c r="A67" s="10"/>
+      <c r="B67" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="13" t="s">
+    <row r="68" spans="1:2">
+      <c r="A68" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B68" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="14"/>
-      <c r="B68" s="4" t="s">
+    <row r="69" spans="1:2">
+      <c r="A69" s="12"/>
+      <c r="B69" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="14"/>
-      <c r="B69" s="4" t="s">
+    <row r="70" spans="1:2">
+      <c r="A70" s="12"/>
+      <c r="B70" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="14"/>
-      <c r="B70" s="4" t="s">
+    <row r="71" spans="1:2">
+      <c r="A71" s="12"/>
+      <c r="B71" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
-      <c r="A71" s="14"/>
-      <c r="B71" s="4" t="s">
+    <row r="72" spans="1:2">
+      <c r="A72" s="12"/>
+      <c r="B72" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
-      <c r="A72" s="14"/>
-      <c r="B72" s="4" t="s">
+    <row r="73" spans="1:2">
+      <c r="A73" s="12"/>
+      <c r="B73" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="14"/>
-      <c r="B73" s="4" t="s">
+    <row r="74" spans="1:2">
+      <c r="A74" s="12"/>
+      <c r="B74" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
-      <c r="A74" s="14"/>
-      <c r="B74" s="4" t="s">
+    <row r="75" spans="1:2">
+      <c r="A75" s="12"/>
+      <c r="B75" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
-      <c r="A75" s="14"/>
-      <c r="B75" s="4" t="s">
+    <row r="76" spans="1:2">
+      <c r="A76" s="12"/>
+      <c r="B76" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
-      <c r="A76" s="15"/>
-      <c r="B76" s="3" t="s">
+    <row r="77" spans="1:2">
+      <c r="A77" s="13"/>
+      <c r="B77" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
-      <c r="A77" s="16" t="s">
+    <row r="78" spans="1:2">
+      <c r="A78" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B78" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
-      <c r="A78" s="17"/>
-      <c r="B78" s="3" t="s">
+    <row r="79" spans="1:2">
+      <c r="A79" s="15"/>
+      <c r="B79" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
-      <c r="A79" s="18"/>
-      <c r="B79" s="3" t="s">
+    <row r="80" spans="1:2">
+      <c r="A80" s="16"/>
+      <c r="B80" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
-      <c r="A80" s="13" t="s">
+    <row r="81" spans="1:2">
+      <c r="A81" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B81" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="15"/>
-      <c r="B81" s="3" t="s">
+    <row r="82" spans="1:2">
+      <c r="A82" s="13"/>
+      <c r="B82" s="3" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>70</v>
@@ -1397,7 +1398,7 @@
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>70</v>
@@ -1405,29 +1406,37 @@
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>70</v>
       </c>
     </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A64:A66"/>
-    <mergeCell ref="A67:A76"/>
-    <mergeCell ref="A77:A79"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A80:A81"/>
-    <mergeCell ref="A34:A41"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="A45:A49"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A58:A63"/>
     <mergeCell ref="A2:A9"/>
     <mergeCell ref="A10:A14"/>
     <mergeCell ref="A15:A23"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A34:A41"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A45:A49"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A59:A64"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="A68:A77"/>
+    <mergeCell ref="A78:A80"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="A81:A82"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
collections modified and frozen set added
</commit_message>
<xml_diff>
--- a/python_syllabus.xlsx
+++ b/python_syllabus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\pythontraining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722B7246-C709-4072-AB0B-59D1F3952241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF36A5B7-248C-4085-8094-C40397952F20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="112">
   <si>
     <t>Topic</t>
   </si>
@@ -241,12 +241,6 @@
     <t>Network Programming</t>
   </si>
   <si>
-    <t>Tkinter</t>
-  </si>
-  <si>
-    <t>DJANGO ESSENTIAL</t>
-  </si>
-  <si>
     <t>sort_vs_sorted.py</t>
   </si>
   <si>
@@ -286,76 +280,101 @@
     <t>class_oops.py</t>
   </si>
   <si>
-    <t>polymorphism.py (overloading | overriding)</t>
+    <t>Decorator / Iterator / Generator</t>
+  </si>
+  <si>
+    <t>counters.py</t>
+  </si>
+  <si>
+    <t>ordereddict.py</t>
+  </si>
+  <si>
+    <t>defaultdict.py</t>
+  </si>
+  <si>
+    <t>chainmap.py</t>
+  </si>
+  <si>
+    <t>namedtuple.py</t>
+  </si>
+  <si>
+    <t>deque.py</t>
+  </si>
+  <si>
+    <t>userdict.py</t>
+  </si>
+  <si>
+    <t>userlist.py</t>
+  </si>
+  <si>
+    <t>userstring.py</t>
+  </si>
+  <si>
+    <t>ordereddict_delete_insert.py</t>
+  </si>
+  <si>
+    <t>lambda_function.py</t>
+  </si>
+  <si>
+    <t>map_function.py</t>
+  </si>
+  <si>
+    <t>reduce_function.py</t>
+  </si>
+  <si>
+    <t>filter_function.py</t>
+  </si>
+  <si>
+    <t>threading.py</t>
+  </si>
+  <si>
+    <t>thread_details.py</t>
+  </si>
+  <si>
+    <t>named_parameters.py</t>
+  </si>
+  <si>
+    <t>DB Connection</t>
+  </si>
+  <si>
+    <t>db_access.py</t>
+  </si>
+  <si>
+    <t>frozen_set.py</t>
   </si>
   <si>
     <t>Map / Reduce / Filter</t>
   </si>
   <si>
-    <t>Decorator / Iterator / Generator</t>
-  </si>
-  <si>
-    <t>counters.py</t>
-  </si>
-  <si>
-    <t>ordereddict.py</t>
-  </si>
-  <si>
-    <t>defaultdict.py</t>
-  </si>
-  <si>
-    <t>chainmap.py</t>
-  </si>
-  <si>
-    <t>namedtuple.py</t>
-  </si>
-  <si>
-    <t>deque.py</t>
-  </si>
-  <si>
-    <t>userdict.py</t>
-  </si>
-  <si>
-    <t>userlist.py</t>
-  </si>
-  <si>
-    <t>userstring.py</t>
-  </si>
-  <si>
-    <t>ordereddict_delete_insert.py</t>
-  </si>
-  <si>
-    <t>lambda_function.py</t>
-  </si>
-  <si>
-    <t>map_function.py</t>
-  </si>
-  <si>
-    <t>reduce_function.py</t>
-  </si>
-  <si>
-    <t>filter_function.py</t>
-  </si>
-  <si>
-    <t>threading.py</t>
-  </si>
-  <si>
-    <t>thread_details.py</t>
-  </si>
-  <si>
-    <t>named_parameters.py</t>
+    <t>method_overloading</t>
+  </si>
+  <si>
+    <t>namedtuple - tuple of tuple</t>
+  </si>
+  <si>
+    <t>polymorphism.py ( medthod overloading/overriding )</t>
+  </si>
+  <si>
+    <t>Django Essential / Pattern</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -373,23 +392,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -512,59 +514,53 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -841,17 +837,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B86"/>
+  <dimension ref="A1:D87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B58" sqref="B58"/>
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="33.1796875" customWidth="1"/>
-    <col min="2" max="2" width="37.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -863,7 +860,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -871,49 +868,49 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="17"/>
+      <c r="A3" s="6"/>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="17"/>
+      <c r="A4" s="6"/>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="17"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="17"/>
+      <c r="A6" s="6"/>
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="17"/>
-      <c r="B7" s="7" t="s">
+      <c r="A7" s="6"/>
+      <c r="B7" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="17"/>
-      <c r="B8" s="7" t="s">
-        <v>78</v>
+      <c r="A8" s="6"/>
+      <c r="B8" s="14" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="17"/>
-      <c r="B9" s="7" t="s">
-        <v>85</v>
+      <c r="A9" s="6"/>
+      <c r="B9" s="14" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -921,31 +918,31 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="17"/>
+      <c r="A11" s="6"/>
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="17"/>
+      <c r="A12" s="6"/>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="17"/>
+      <c r="A13" s="6"/>
       <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="17"/>
+      <c r="A14" s="6"/>
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -953,55 +950,55 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="17"/>
+      <c r="A16" s="6"/>
       <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="17"/>
+      <c r="A17" s="6"/>
       <c r="B17" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="17"/>
+      <c r="A18" s="6"/>
       <c r="B18" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="17"/>
+      <c r="A19" s="6"/>
       <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="17"/>
+      <c r="A20" s="6"/>
       <c r="B20" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="17"/>
+      <c r="A21" s="6"/>
       <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="17"/>
+      <c r="A22" s="6"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="17"/>
+      <c r="A23" s="6"/>
       <c r="B23" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1009,19 +1006,19 @@
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="17"/>
+      <c r="A25" s="6"/>
       <c r="B25" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="17"/>
+      <c r="A26" s="6"/>
       <c r="B26" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1029,15 +1026,15 @@
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="5" t="s">
-        <v>76</v>
+      <c r="A28" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1045,398 +1042,410 @@
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="17"/>
+      <c r="A30" s="6"/>
       <c r="B30" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="17"/>
+      <c r="A31" s="6"/>
       <c r="B31" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="6"/>
+      <c r="B32" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="4"/>
+      <c r="B33" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="6"/>
+      <c r="B36" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="6"/>
+      <c r="B37" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="6"/>
+      <c r="B38" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="17"/>
-      <c r="B32" s="2" t="s">
+    <row r="39" spans="1:2">
+      <c r="A39" s="6"/>
+      <c r="B39" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="6"/>
+      <c r="B40" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="17"/>
-      <c r="B35" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="17"/>
-      <c r="B36" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="17"/>
-      <c r="B37" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="17"/>
-      <c r="B38" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="17"/>
-      <c r="B39" s="2" t="s">
+    <row r="41" spans="1:2">
+      <c r="A41" s="6"/>
+      <c r="B41" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="6"/>
+      <c r="B42" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="7"/>
+      <c r="B44" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="7"/>
+      <c r="B45" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="7"/>
+      <c r="B47" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="7"/>
+      <c r="B48" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="7"/>
+      <c r="B49" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="7"/>
+      <c r="B50" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="7"/>
+      <c r="B53" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="7"/>
+      <c r="B54" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="7"/>
+      <c r="B55" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B56" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="12"/>
+      <c r="B58" s="15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="13"/>
+      <c r="B59" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B60" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="7"/>
+      <c r="B61" s="15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="7"/>
+      <c r="B62" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="7"/>
+      <c r="B63" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="7"/>
+      <c r="B64" s="15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="7"/>
+      <c r="B65" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B66" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="9"/>
+      <c r="B67" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="10"/>
+      <c r="B68" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B69" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="9"/>
+      <c r="B70" s="15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="9"/>
+      <c r="B71" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="9"/>
+      <c r="B72" s="15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="9"/>
+      <c r="B73" s="15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="9"/>
+      <c r="B74" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="9"/>
+      <c r="B75" s="15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="9"/>
+      <c r="B76" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="9"/>
+      <c r="B77" s="15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="10"/>
+      <c r="B78" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B79" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="D79" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="12"/>
+      <c r="B80" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D80" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="12"/>
+      <c r="B81" s="15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="8" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="17"/>
-      <c r="B40" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="17"/>
-      <c r="B41" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="18"/>
-      <c r="B43" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="18"/>
-      <c r="B44" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="18"/>
-      <c r="B46" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="18"/>
-      <c r="B47" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="18"/>
-      <c r="B48" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="18"/>
-      <c r="B49" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="18"/>
-      <c r="B52" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="18"/>
-      <c r="B53" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="18"/>
-      <c r="B54" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="15"/>
-      <c r="B57" s="3" t="s">
+      <c r="B82" s="15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="16"/>
-      <c r="B58" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="18"/>
-      <c r="B60" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="18"/>
-      <c r="B61" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="18"/>
-      <c r="B62" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="18"/>
-      <c r="B63" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="18"/>
-      <c r="B64" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="9"/>
-      <c r="B66" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="10"/>
-      <c r="B67" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="12"/>
-      <c r="B69" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="12"/>
-      <c r="B70" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
-      <c r="A71" s="12"/>
-      <c r="B71" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
-      <c r="A72" s="12"/>
-      <c r="B72" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="12"/>
-      <c r="B73" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
-      <c r="A74" s="12"/>
-      <c r="B74" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
-      <c r="A75" s="12"/>
-      <c r="B75" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
-      <c r="A76" s="12"/>
-      <c r="B76" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="A77" s="13"/>
-      <c r="B77" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
-      <c r="A78" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="B78" s="3" t="s">
+    <row r="83" spans="1:2">
+      <c r="A83" s="10"/>
+      <c r="B83" s="15" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
-      <c r="A79" s="15"/>
-      <c r="B79" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2">
-      <c r="A80" s="16"/>
-      <c r="B80" s="3" t="s">
+    <row r="84" spans="1:2">
+      <c r="A84" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="B81" s="3" t="s">
+      <c r="B84" s="15" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="13"/>
-      <c r="B82" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="6" t="s">
+    <row r="85" spans="1:2">
+      <c r="A85" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B85" s="15" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="6" t="s">
+    <row r="86" spans="1:2">
+      <c r="A86" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B86" s="15" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
-      <c r="A85" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
-      <c r="A86" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B86" s="3" t="s">
+    <row r="87" spans="1:2">
+      <c r="A87" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B87" s="15" t="s">
         <v>70</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="A69:A78"/>
+    <mergeCell ref="A79:A81"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="A46:A50"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="A60:A65"/>
     <mergeCell ref="A2:A9"/>
     <mergeCell ref="A10:A14"/>
     <mergeCell ref="A15:A23"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A34:A41"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="A45:A49"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A59:A64"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="A68:A77"/>
-    <mergeCell ref="A78:A80"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="A81:A82"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Map Filter Reduce & Threading refined
</commit_message>
<xml_diff>
--- a/python_syllabus.xlsx
+++ b/python_syllabus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\pythontraining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF36A5B7-248C-4085-8094-C40397952F20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09C9501-AFD9-477B-9931-ED8261CA23C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -325,9 +325,6 @@
     <t>filter_function.py</t>
   </si>
   <si>
-    <t>threading.py</t>
-  </si>
-  <si>
     <t>thread_details.py</t>
   </si>
   <si>
@@ -356,18 +353,28 @@
   </si>
   <si>
     <t>Django Essential / Pattern</t>
+  </si>
+  <si>
+    <t>thread.py</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -514,53 +521,56 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -840,8 +850,8 @@
   <dimension ref="A1:D87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -860,7 +870,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="15" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -868,49 +878,49 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="6"/>
+      <c r="A3" s="15"/>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="6"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="6"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="6"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="14" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="14" t="s">
+      <c r="A8" s="15"/>
+      <c r="B8" s="6" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="14" t="s">
+      <c r="A9" s="15"/>
+      <c r="B9" s="6" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="15" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -918,31 +928,31 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="6"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="6"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="6"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="6"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="15" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -950,55 +960,55 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="6"/>
+      <c r="A16" s="15"/>
       <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="6"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="6"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="6"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="6"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="6"/>
+      <c r="A21" s="15"/>
       <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="6"/>
+      <c r="A22" s="15"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="6"/>
+      <c r="A23" s="15"/>
       <c r="B23" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1006,13 +1016,13 @@
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="6"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="6"/>
+      <c r="A26" s="15"/>
       <c r="B26" s="2" t="s">
         <v>27</v>
       </c>
@@ -1034,7 +1044,7 @@
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="15" t="s">
         <v>30</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1042,19 +1052,19 @@
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="6"/>
+      <c r="A30" s="15"/>
       <c r="B30" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="6"/>
+      <c r="A31" s="15"/>
       <c r="B31" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="6"/>
+      <c r="A32" s="15"/>
       <c r="B32" s="2" t="s">
         <v>80</v>
       </c>
@@ -1070,11 +1080,11 @@
         <v>77</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -1082,49 +1092,49 @@
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="6"/>
+      <c r="A36" s="15"/>
       <c r="B36" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="6"/>
+      <c r="A37" s="15"/>
       <c r="B37" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="6"/>
+      <c r="A38" s="15"/>
       <c r="B38" s="2" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="6"/>
+      <c r="A39" s="15"/>
       <c r="B39" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="6"/>
+      <c r="A40" s="15"/>
       <c r="B40" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="6"/>
+      <c r="A41" s="15"/>
       <c r="B41" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="6"/>
+      <c r="A42" s="15"/>
       <c r="B42" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="16" t="s">
         <v>40</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -1132,19 +1142,19 @@
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="7"/>
+      <c r="A44" s="16"/>
       <c r="B44" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="7"/>
+      <c r="A45" s="16"/>
       <c r="B45" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="16" t="s">
         <v>44</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -1152,26 +1162,26 @@
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="7"/>
-      <c r="B47" s="15" t="s">
+      <c r="A47" s="16"/>
+      <c r="B47" s="7" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="7"/>
-      <c r="B48" s="15" t="s">
+      <c r="A48" s="16"/>
+      <c r="B48" s="7" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="7"/>
-      <c r="B49" s="15" t="s">
+      <c r="A49" s="16"/>
+      <c r="B49" s="7" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50" s="7"/>
-      <c r="B50" s="15" t="s">
+      <c r="A50" s="16"/>
+      <c r="B50" s="7" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1179,33 +1189,33 @@
       <c r="A51" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B52" s="15" t="s">
+      <c r="B52" s="7" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="7"/>
-      <c r="B53" s="15" t="s">
+      <c r="A53" s="16"/>
+      <c r="B53" s="7" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="7"/>
-      <c r="B54" s="15" t="s">
+      <c r="A54" s="16"/>
+      <c r="B54" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="7"/>
-      <c r="B55" s="15" t="s">
+      <c r="A55" s="16"/>
+      <c r="B55" s="7" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1213,203 +1223,203 @@
       <c r="A56" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="15" t="s">
+      <c r="B56" s="7" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:2">
-      <c r="A57" s="11" t="s">
+      <c r="A57" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="15" t="s">
+      <c r="B57" s="7" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:2">
-      <c r="A58" s="12"/>
-      <c r="B58" s="15" t="s">
+      <c r="A58" s="13"/>
+      <c r="B58" s="7" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="13"/>
-      <c r="B59" s="15" t="s">
-        <v>103</v>
+      <c r="A59" s="14"/>
+      <c r="B59" s="7" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="60" spans="1:2">
-      <c r="A60" s="7" t="s">
+      <c r="A60" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B60" s="15" t="s">
+      <c r="B60" s="7" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="61" spans="1:2">
-      <c r="A61" s="7"/>
-      <c r="B61" s="15" t="s">
+      <c r="A61" s="16"/>
+      <c r="B61" s="7" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="62" spans="1:2">
-      <c r="A62" s="7"/>
-      <c r="B62" s="15" t="s">
+      <c r="A62" s="16"/>
+      <c r="B62" s="7" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="63" spans="1:2">
-      <c r="A63" s="7"/>
-      <c r="B63" s="15" t="s">
+      <c r="A63" s="16"/>
+      <c r="B63" s="7" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="7"/>
-      <c r="B64" s="15" t="s">
-        <v>110</v>
+      <c r="A64" s="16"/>
+      <c r="B64" s="7" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="7"/>
-      <c r="B65" s="15" t="s">
+      <c r="A65" s="16"/>
+      <c r="B65" s="7" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="16" t="s">
+      <c r="A66" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B66" s="15" t="s">
+      <c r="B66" s="7" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="9"/>
-      <c r="B67" s="15" t="s">
+      <c r="B67" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="10"/>
-      <c r="B68" s="15" t="s">
+      <c r="B68" s="7" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="69" spans="1:4">
-      <c r="A69" s="8" t="s">
+      <c r="A69" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B69" s="15" t="s">
+      <c r="B69" s="7" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="9"/>
-      <c r="B70" s="15" t="s">
+      <c r="B70" s="7" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="9"/>
-      <c r="B71" s="15" t="s">
+      <c r="B71" s="7" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="9"/>
-      <c r="B72" s="15" t="s">
+      <c r="B72" s="7" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="9"/>
-      <c r="B73" s="15" t="s">
+      <c r="B73" s="7" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="9"/>
-      <c r="B74" s="15" t="s">
+      <c r="B74" s="7" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="9"/>
-      <c r="B75" s="15" t="s">
+      <c r="B75" s="7" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="9"/>
-      <c r="B76" s="15" t="s">
+      <c r="B76" s="7" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="9"/>
-      <c r="B77" s="15" t="s">
+      <c r="B77" s="7" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="10"/>
-      <c r="B78" s="15" t="s">
+      <c r="B78" s="7" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="79" spans="1:4">
-      <c r="A79" s="11" t="s">
+      <c r="A79" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D79" t="s">
         <v>107</v>
       </c>
-      <c r="B79" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="D79" t="s">
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="13"/>
+      <c r="B80" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D80" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="12"/>
-      <c r="B80" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="D80" t="s">
-        <v>109</v>
-      </c>
-    </row>
     <row r="81" spans="1:2">
-      <c r="A81" s="12"/>
-      <c r="B81" s="15" t="s">
+      <c r="A81" s="13"/>
+      <c r="B81" s="7" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="82" spans="1:2">
-      <c r="A82" s="8" t="s">
+      <c r="A82" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B82" s="15" t="s">
-        <v>101</v>
+      <c r="B82" s="17" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="10"/>
-      <c r="B83" s="15" t="s">
-        <v>102</v>
+      <c r="B83" s="7" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B84" s="7" t="s">
         <v>104</v>
-      </c>
-      <c r="B84" s="15" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B85" s="15" t="s">
+      <c r="B85" s="7" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1417,35 +1427,35 @@
       <c r="A86" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B86" s="15" t="s">
+      <c r="B86" s="7" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B87" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B87" s="7" t="s">
         <v>70</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A15:A23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="A46:A50"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="A60:A65"/>
     <mergeCell ref="A66:A68"/>
     <mergeCell ref="A69:A78"/>
     <mergeCell ref="A79:A81"/>
     <mergeCell ref="A57:A59"/>
     <mergeCell ref="A82:A83"/>
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="A46:A50"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="A60:A65"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A15:A23"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A29:A32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
DB programs added and introduction refined
</commit_message>
<xml_diff>
--- a/python_syllabus.xlsx
+++ b/python_syllabus.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\pythontraining\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09C9501-AFD9-477B-9931-ED8261CA23C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5F6954-5996-427B-9C8F-8C4571EA9B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="115">
   <si>
     <t>Topic</t>
   </si>
@@ -334,21 +334,12 @@
     <t>DB Connection</t>
   </si>
   <si>
-    <t>db_access.py</t>
-  </si>
-  <si>
     <t>frozen_set.py</t>
   </si>
   <si>
     <t>Map / Reduce / Filter</t>
   </si>
   <si>
-    <t>method_overloading</t>
-  </si>
-  <si>
-    <t>namedtuple - tuple of tuple</t>
-  </si>
-  <si>
     <t>polymorphism.py ( medthod overloading/overriding )</t>
   </si>
   <si>
@@ -356,6 +347,24 @@
   </si>
   <si>
     <t>thread.py</t>
+  </si>
+  <si>
+    <t>create_table.py</t>
+  </si>
+  <si>
+    <t>delete_table_values.py</t>
+  </si>
+  <si>
+    <t>insert_values_into_table.py</t>
+  </si>
+  <si>
+    <t>mysql_version_finding.py</t>
+  </si>
+  <si>
+    <t>read_table_values.py</t>
+  </si>
+  <si>
+    <t>update_table_values.py</t>
   </si>
 </sst>
 </file>
@@ -521,15 +530,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -540,6 +546,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -561,15 +576,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -847,18 +853,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D87"/>
+  <dimension ref="A1:B92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B87" sqref="B87"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="33.1796875" customWidth="1"/>
     <col min="2" max="2" width="46.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -870,7 +875,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -878,49 +883,49 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="15"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="15"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="15"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="15"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="15"/>
-      <c r="B7" s="6" t="s">
+      <c r="A7" s="8"/>
+      <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="15"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="8"/>
+      <c r="B8" s="5" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="15"/>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="8"/>
+      <c r="B9" s="5" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -928,31 +933,31 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="15"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="15"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="15"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="15"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -960,55 +965,55 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="15"/>
+      <c r="A16" s="8"/>
       <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="15"/>
+      <c r="A17" s="8"/>
       <c r="B17" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="15"/>
+      <c r="A18" s="8"/>
       <c r="B18" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="15"/>
+      <c r="A19" s="8"/>
       <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="15"/>
+      <c r="A20" s="8"/>
       <c r="B20" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="15"/>
+      <c r="A21" s="8"/>
       <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="15"/>
+      <c r="A22" s="8"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="15"/>
+      <c r="A23" s="8"/>
       <c r="B23" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1016,19 +1021,19 @@
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="15"/>
+      <c r="A25" s="8"/>
       <c r="B25" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="15"/>
+      <c r="A26" s="8"/>
       <c r="B26" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1036,7 +1041,7 @@
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -1044,7 +1049,7 @@
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1052,39 +1057,39 @@
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="15"/>
+      <c r="A30" s="8"/>
       <c r="B30" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="15"/>
+      <c r="A31" s="8"/>
       <c r="B31" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="15"/>
+      <c r="A32" s="8"/>
       <c r="B32" s="2" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="4"/>
+      <c r="A33" s="3"/>
       <c r="B33" s="2" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="3" t="s">
         <v>77</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="8" t="s">
         <v>33</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -1092,49 +1097,49 @@
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="15"/>
+      <c r="A36" s="8"/>
       <c r="B36" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="15"/>
+      <c r="A37" s="8"/>
       <c r="B37" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="15"/>
+      <c r="A38" s="8"/>
       <c r="B38" s="2" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="15"/>
+      <c r="A39" s="8"/>
       <c r="B39" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="15"/>
+      <c r="A40" s="8"/>
       <c r="B40" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="15"/>
+      <c r="A41" s="8"/>
       <c r="B41" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="15"/>
+      <c r="A42" s="8"/>
       <c r="B42" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="16" t="s">
+      <c r="A43" s="9" t="s">
         <v>40</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -1142,19 +1147,19 @@
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="16"/>
+      <c r="A44" s="9"/>
       <c r="B44" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="16"/>
+      <c r="A45" s="9"/>
       <c r="B45" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="16" t="s">
+      <c r="A46" s="9" t="s">
         <v>44</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -1162,300 +1167,325 @@
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="16"/>
-      <c r="B47" s="7" t="s">
+      <c r="A47" s="9"/>
+      <c r="B47" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="16"/>
-      <c r="B48" s="7" t="s">
+      <c r="A48" s="9"/>
+      <c r="B48" s="6" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="16"/>
-      <c r="B49" s="7" t="s">
+      <c r="A49" s="9"/>
+      <c r="B49" s="6" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50" s="16"/>
-      <c r="B50" s="7" t="s">
+      <c r="A50" s="9"/>
+      <c r="B50" s="6" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:2">
-      <c r="A51" s="5" t="s">
+      <c r="A51" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="6" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" s="16" t="s">
+      <c r="A52" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="16"/>
-      <c r="B53" s="7" t="s">
+      <c r="A53" s="9"/>
+      <c r="B53" s="6" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="16"/>
-      <c r="B54" s="7" t="s">
+      <c r="A54" s="9"/>
+      <c r="B54" s="6" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="16"/>
-      <c r="B55" s="7" t="s">
+      <c r="A55" s="9"/>
+      <c r="B55" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B56" s="6" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:2">
-      <c r="A57" s="12" t="s">
+      <c r="A57" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B57" s="6" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:2">
-      <c r="A58" s="13"/>
-      <c r="B58" s="7" t="s">
+      <c r="A58" s="15"/>
+      <c r="B58" s="6" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="14"/>
-      <c r="B59" s="7" t="s">
+      <c r="A59" s="16"/>
+      <c r="B59" s="6" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="60" spans="1:2">
-      <c r="A60" s="16" t="s">
+      <c r="A60" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B60" s="6" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="61" spans="1:2">
-      <c r="A61" s="16"/>
-      <c r="B61" s="7" t="s">
+      <c r="A61" s="9"/>
+      <c r="B61" s="6" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="62" spans="1:2">
-      <c r="A62" s="16"/>
-      <c r="B62" s="7" t="s">
+      <c r="A62" s="9"/>
+      <c r="B62" s="6" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="63" spans="1:2">
-      <c r="A63" s="16"/>
-      <c r="B63" s="7" t="s">
+      <c r="A63" s="9"/>
+      <c r="B63" s="6" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="16"/>
-      <c r="B64" s="7" t="s">
+      <c r="A64" s="9"/>
+      <c r="B64" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="9"/>
+      <c r="B65" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="11"/>
+      <c r="B67" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="12"/>
+      <c r="B68" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="11"/>
+      <c r="B70" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="11"/>
+      <c r="B71" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="11"/>
+      <c r="B72" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="11"/>
+      <c r="B73" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="11"/>
+      <c r="B74" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="11"/>
+      <c r="B75" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="11"/>
+      <c r="B76" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="11"/>
+      <c r="B77" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="12"/>
+      <c r="B78" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="15"/>
+      <c r="B80" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="15"/>
+      <c r="B81" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="12"/>
+      <c r="B83" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="11"/>
+      <c r="B85" s="6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="16"/>
-      <c r="B65" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="9"/>
-      <c r="B67" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="10"/>
-      <c r="B68" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="9"/>
-      <c r="B70" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="9"/>
-      <c r="B71" s="7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="9"/>
-      <c r="B72" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
-      <c r="A73" s="9"/>
-      <c r="B73" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
-      <c r="A74" s="9"/>
-      <c r="B74" s="7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
-      <c r="A75" s="9"/>
-      <c r="B75" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="9"/>
-      <c r="B76" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="9"/>
-      <c r="B77" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="10"/>
-      <c r="B78" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D79" t="s">
+    <row r="86" spans="1:2">
+      <c r="A86" s="11"/>
+      <c r="B86" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="11"/>
+      <c r="B87" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="11"/>
+      <c r="B88" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="12"/>
+      <c r="B89" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="4" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="13"/>
-      <c r="B80" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="D80" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="13"/>
-      <c r="B81" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B82" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="10"/>
-      <c r="B83" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B84" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2">
-      <c r="A85" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B85" s="7" t="s">
+      <c r="B92" s="6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
-      <c r="A86" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2">
-      <c r="A87" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B87" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="A84:A89"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="A69:A78"/>
+    <mergeCell ref="A79:A81"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="A46:A50"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="A60:A65"/>
     <mergeCell ref="A2:A9"/>
     <mergeCell ref="A10:A14"/>
     <mergeCell ref="A15:A23"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="A46:A50"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="A60:A65"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="A69:A78"/>
-    <mergeCell ref="A79:A81"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="A82:A83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Syllabus updated & links deleted
</commit_message>
<xml_diff>
--- a/python_syllabus.xlsx
+++ b/python_syllabus.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5F6954-5996-427B-9C8F-8C4571EA9B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB40A45D-1733-4283-837F-484374F0DD3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Syllabus" sheetId="1" r:id="rId1"/>
+    <sheet name="Links" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="125">
   <si>
     <t>Topic</t>
   </si>
@@ -365,6 +366,36 @@
   </si>
   <si>
     <t>update_table_values.py</t>
+  </si>
+  <si>
+    <t>Syllabus</t>
+  </si>
+  <si>
+    <t>Practicals</t>
+  </si>
+  <si>
+    <t>API's</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/introduction-to-apis/</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/python-network-programming/</t>
+  </si>
+  <si>
+    <t>Tkinter</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/python-gui-tkinter/</t>
+  </si>
+  <si>
+    <t>Django</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/django-tutorial/</t>
+  </si>
+  <si>
+    <t>URL</t>
   </si>
 </sst>
 </file>
@@ -415,7 +446,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -434,8 +465,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -497,29 +534,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <right/>
       <top/>
       <bottom style="thin">
         <color auto="1"/>
@@ -530,18 +545,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -557,8 +566,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -566,17 +587,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -853,641 +871,708 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B92"/>
+  <dimension ref="A1:E87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="33.1796875" customWidth="1"/>
+    <col min="1" max="1" width="28.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.1796875" customWidth="1"/>
+    <col min="4" max="4" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="D1" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="8" t="s">
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="8"/>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="10"/>
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="8"/>
-      <c r="B4" s="2" t="s">
+      <c r="D4" s="13"/>
+      <c r="E4" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="10"/>
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="8"/>
-      <c r="B5" s="2" t="s">
+      <c r="D5" s="13"/>
+      <c r="E5" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="10"/>
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="2" t="s">
+      <c r="D6" s="13"/>
+      <c r="E6" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="10"/>
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="5" t="s">
+      <c r="D7" s="13"/>
+      <c r="E7" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="10"/>
+      <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="5" t="s">
+      <c r="D8" s="14"/>
+      <c r="E8" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="10"/>
+      <c r="B9" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="5" t="s">
+    <row r="10" spans="1:5">
+      <c r="A10" s="10"/>
+      <c r="B10" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="8" t="s">
+    <row r="11" spans="1:5">
+      <c r="A11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="8"/>
-      <c r="B11" s="2" t="s">
+    <row r="12" spans="1:5">
+      <c r="A12" s="10"/>
+      <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="2" t="s">
+    <row r="13" spans="1:5">
+      <c r="A13" s="10"/>
+      <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="8"/>
-      <c r="B13" s="2" t="s">
+    <row r="14" spans="1:5">
+      <c r="A14" s="10"/>
+      <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="2" t="s">
+    <row r="15" spans="1:5">
+      <c r="A15" s="10"/>
+      <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="8" t="s">
+    <row r="16" spans="1:5">
+      <c r="A16" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="8"/>
-      <c r="B16" s="2" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17" s="10"/>
+      <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="8"/>
-      <c r="B17" s="2" t="s">
+    <row r="18" spans="1:2">
+      <c r="A18" s="10"/>
+      <c r="B18" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="8"/>
-      <c r="B18" s="2" t="s">
+    <row r="19" spans="1:2">
+      <c r="A19" s="10"/>
+      <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="8"/>
-      <c r="B19" s="2" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" s="10"/>
+      <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="8"/>
-      <c r="B20" s="2" t="s">
+    <row r="21" spans="1:2">
+      <c r="A21" s="10"/>
+      <c r="B21" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="8"/>
-      <c r="B21" s="2" t="s">
+    <row r="22" spans="1:2">
+      <c r="A22" s="10"/>
+      <c r="B22" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="8"/>
-      <c r="B22" s="2" t="s">
+    <row r="23" spans="1:2">
+      <c r="A23" s="10"/>
+      <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="8"/>
-      <c r="B23" s="2" t="s">
+    <row r="24" spans="1:2">
+      <c r="A24" s="10"/>
+      <c r="B24" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="8" t="s">
+    <row r="25" spans="1:2">
+      <c r="A25" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="8"/>
-      <c r="B25" s="2" t="s">
+    <row r="26" spans="1:2">
+      <c r="A26" s="10"/>
+      <c r="B26" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="8"/>
-      <c r="B26" s="2" t="s">
+    <row r="27" spans="1:2">
+      <c r="A27" s="10"/>
+      <c r="B27" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="3" t="s">
+    <row r="28" spans="1:2">
+      <c r="A28" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="3" t="s">
+    <row r="29" spans="1:2">
+      <c r="A29" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="8" t="s">
+    <row r="30" spans="1:2">
+      <c r="A30" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="8"/>
-      <c r="B30" s="2" t="s">
+    <row r="31" spans="1:2">
+      <c r="A31" s="10"/>
+      <c r="B31" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="8"/>
-      <c r="B31" s="2" t="s">
+    <row r="32" spans="1:2">
+      <c r="A32" s="10"/>
+      <c r="B32" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="8"/>
-      <c r="B32" s="2" t="s">
+    <row r="33" spans="1:2">
+      <c r="A33" s="10"/>
+      <c r="B33" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="3"/>
-      <c r="B33" s="2" t="s">
+    <row r="34" spans="1:2">
+      <c r="A34" s="6"/>
+      <c r="B34" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="3" t="s">
+    <row r="35" spans="1:2">
+      <c r="A35" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="8" t="s">
+    <row r="36" spans="1:2">
+      <c r="A36" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="8"/>
-      <c r="B36" s="2" t="s">
+    <row r="37" spans="1:2">
+      <c r="A37" s="10"/>
+      <c r="B37" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="8"/>
-      <c r="B37" s="2" t="s">
+    <row r="38" spans="1:2">
+      <c r="A38" s="10"/>
+      <c r="B38" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="8"/>
-      <c r="B38" s="2" t="s">
+    <row r="39" spans="1:2">
+      <c r="A39" s="10"/>
+      <c r="B39" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="8"/>
-      <c r="B39" s="2" t="s">
+    <row r="40" spans="1:2">
+      <c r="A40" s="10"/>
+      <c r="B40" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="8"/>
-      <c r="B40" s="2" t="s">
+    <row r="41" spans="1:2">
+      <c r="A41" s="10"/>
+      <c r="B41" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="8"/>
-      <c r="B41" s="2" t="s">
+    <row r="42" spans="1:2">
+      <c r="A42" s="10"/>
+      <c r="B42" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="8"/>
-      <c r="B42" s="2" t="s">
+    <row r="43" spans="1:2">
+      <c r="A43" s="10"/>
+      <c r="B43" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="9" t="s">
+    <row r="44" spans="1:2">
+      <c r="A44" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="9"/>
-      <c r="B44" s="2" t="s">
+    <row r="45" spans="1:2">
+      <c r="A45" s="11"/>
+      <c r="B45" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="9"/>
-      <c r="B45" s="2" t="s">
+    <row r="46" spans="1:2">
+      <c r="A46" s="11"/>
+      <c r="B46" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="9" t="s">
+    <row r="47" spans="1:2">
+      <c r="A47" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="9"/>
-      <c r="B47" s="6" t="s">
+    <row r="48" spans="1:2">
+      <c r="A48" s="11"/>
+      <c r="B48" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="9"/>
-      <c r="B48" s="6" t="s">
+    <row r="49" spans="1:2">
+      <c r="A49" s="11"/>
+      <c r="B49" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="9"/>
-      <c r="B49" s="6" t="s">
+    <row r="50" spans="1:2">
+      <c r="A50" s="11"/>
+      <c r="B50" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="9"/>
-      <c r="B50" s="6" t="s">
+    <row r="51" spans="1:2">
+      <c r="A51" s="11"/>
+      <c r="B51" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="4" t="s">
+    <row r="52" spans="1:2">
+      <c r="A52" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B52" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="9" t="s">
+    <row r="53" spans="1:2">
+      <c r="A53" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B53" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="9"/>
-      <c r="B53" s="6" t="s">
+    <row r="54" spans="1:2">
+      <c r="A54" s="11"/>
+      <c r="B54" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="9"/>
-      <c r="B54" s="6" t="s">
+    <row r="55" spans="1:2">
+      <c r="A55" s="11"/>
+      <c r="B55" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="9"/>
-      <c r="B55" s="6" t="s">
+    <row r="56" spans="1:2">
+      <c r="A56" s="11"/>
+      <c r="B56" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="4" t="s">
+    <row r="57" spans="1:2">
+      <c r="A57" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B57" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="14" t="s">
+    <row r="58" spans="1:2">
+      <c r="A58" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B58" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="15"/>
-      <c r="B58" s="6" t="s">
+    <row r="59" spans="1:2">
+      <c r="A59" s="11"/>
+      <c r="B59" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="16"/>
-      <c r="B59" s="6" t="s">
+    <row r="60" spans="1:2">
+      <c r="A60" s="11"/>
+      <c r="B60" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="9" t="s">
+    <row r="61" spans="1:2">
+      <c r="A61" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="B61" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="9"/>
-      <c r="B61" s="6" t="s">
+    <row r="62" spans="1:2">
+      <c r="A62" s="11"/>
+      <c r="B62" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="9"/>
-      <c r="B62" s="6" t="s">
+    <row r="63" spans="1:2">
+      <c r="A63" s="11"/>
+      <c r="B63" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="9"/>
-      <c r="B63" s="6" t="s">
+    <row r="64" spans="1:2">
+      <c r="A64" s="11"/>
+      <c r="B64" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="9"/>
-      <c r="B64" s="6" t="s">
+    <row r="65" spans="1:2">
+      <c r="A65" s="11"/>
+      <c r="B65" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="9"/>
-      <c r="B65" s="6" t="s">
+    <row r="66" spans="1:2">
+      <c r="A66" s="11"/>
+      <c r="B66" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="10" t="s">
+    <row r="67" spans="1:2">
+      <c r="A67" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="B66" s="6" t="s">
+      <c r="B67" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="11"/>
-      <c r="B67" s="6" t="s">
+    <row r="68" spans="1:2">
+      <c r="A68" s="11"/>
+      <c r="B68" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="12"/>
-      <c r="B68" s="6" t="s">
+    <row r="69" spans="1:2">
+      <c r="A69" s="11"/>
+      <c r="B69" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="13" t="s">
+    <row r="70" spans="1:2">
+      <c r="A70" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B69" s="6" t="s">
+      <c r="B70" s="4" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="11"/>
-      <c r="B70" s="6" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="11"/>
-      <c r="B71" s="6" t="s">
-        <v>96</v>
+      <c r="B71" s="4" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="11"/>
-      <c r="B72" s="6" t="s">
-        <v>89</v>
+      <c r="B72" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="11"/>
-      <c r="B73" s="6" t="s">
-        <v>90</v>
+      <c r="B73" s="4" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="11"/>
-      <c r="B74" s="6" t="s">
-        <v>91</v>
+      <c r="B74" s="4" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="11"/>
-      <c r="B75" s="6" t="s">
-        <v>92</v>
+      <c r="B75" s="4" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="11"/>
-      <c r="B76" s="6" t="s">
-        <v>93</v>
+      <c r="B76" s="4" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="11"/>
-      <c r="B77" s="6" t="s">
+      <c r="B77" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="11"/>
+      <c r="B78" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
-      <c r="A78" s="12"/>
-      <c r="B78" s="6" t="s">
+    <row r="79" spans="1:2">
+      <c r="A79" s="11"/>
+      <c r="B79" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
-      <c r="A79" s="14" t="s">
+    <row r="80" spans="1:2">
+      <c r="A80" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="B79" s="6" t="s">
+      <c r="B80" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
-      <c r="A80" s="15"/>
-      <c r="B80" s="6" t="s">
+    <row r="81" spans="1:2">
+      <c r="A81" s="11"/>
+      <c r="B81" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="15"/>
-      <c r="B81" s="6" t="s">
+    <row r="82" spans="1:2">
+      <c r="A82" s="11"/>
+      <c r="B82" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="13" t="s">
+    <row r="83" spans="1:2">
+      <c r="A83" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B82" s="7" t="s">
+      <c r="B83" s="5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="12"/>
-      <c r="B83" s="6" t="s">
+    <row r="84" spans="1:2">
+      <c r="A84" s="11"/>
+      <c r="B84" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
     <row r="85" spans="1:2">
-      <c r="A85" s="11"/>
-      <c r="B85" s="6" t="s">
-        <v>109</v>
+      <c r="A85" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="86" spans="1:2">
-      <c r="A86" s="11"/>
-      <c r="B86" s="6" t="s">
-        <v>111</v>
+      <c r="A86" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="87" spans="1:2">
-      <c r="A87" s="11"/>
-      <c r="B87" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2">
-      <c r="A88" s="11"/>
-      <c r="B88" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2">
-      <c r="A89" s="12"/>
-      <c r="B89" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2">
-      <c r="A90" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B90" s="6" t="s">
+      <c r="A87" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B87" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
-      <c r="A91" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B91" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="A92" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B92" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A84:A89"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="A69:A78"/>
-    <mergeCell ref="A79:A81"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="A46:A50"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="A60:A65"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A15:A23"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A29:A32"/>
+  <mergeCells count="18">
+    <mergeCell ref="A80:A82"/>
+    <mergeCell ref="A58:A60"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="A61:A66"/>
+    <mergeCell ref="D3:D8"/>
+    <mergeCell ref="A67:A69"/>
+    <mergeCell ref="A70:A79"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A36:A43"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A47:A51"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="A16:A24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25846599-17F5-4659-B5C6-FA28048C5F4C}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
String and list programs modified
</commit_message>
<xml_diff>
--- a/python_syllabus.xlsx
+++ b/python_syllabus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139D82A1-FD39-42EE-A198-1B95023B082C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0893D8F3-681C-4805-852A-D10333F8BD2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,20 @@
     <sheet name="Syllabus" sheetId="1" r:id="rId1"/>
     <sheet name="Links" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -77,9 +90,6 @@
     <t>for_and_in.py</t>
   </si>
   <si>
-    <t>range.py</t>
-  </si>
-  <si>
     <t>while_loop.py</t>
   </si>
   <si>
@@ -396,6 +406,9 @@
   </si>
   <si>
     <t>URL</t>
+  </si>
+  <si>
+    <t>ranges.py</t>
   </si>
 </sst>
 </file>
@@ -591,9 +604,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -601,6 +611,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -880,7 +893,7 @@
   <dimension ref="A1:E87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -895,11 +908,11 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B1" s="10"/>
       <c r="D1" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E1" s="11"/>
     </row>
@@ -925,10 +938,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -938,7 +951,7 @@
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -948,7 +961,7 @@
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -958,7 +971,7 @@
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -968,7 +981,7 @@
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -978,19 +991,19 @@
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="12"/>
       <c r="B9" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="12"/>
       <c r="B10" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1042,461 +1055,461 @@
     <row r="18" spans="1:2">
       <c r="A18" s="12"/>
       <c r="B18" s="2" t="s">
-        <v>18</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="12"/>
       <c r="B19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="12"/>
       <c r="B20" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="12"/>
       <c r="B21" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="12"/>
       <c r="B22" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="12"/>
       <c r="B23" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="12"/>
       <c r="B24" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="12"/>
       <c r="B26" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="12"/>
       <c r="B27" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="12"/>
       <c r="B31" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="12"/>
       <c r="B32" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="12"/>
       <c r="B33" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="18" t="s">
+      <c r="A34" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="19"/>
+      <c r="A35" s="18"/>
       <c r="B35" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="12"/>
       <c r="B37" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="12"/>
       <c r="B38" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="12"/>
       <c r="B39" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="12"/>
       <c r="B40" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="12"/>
       <c r="B41" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="12"/>
       <c r="B42" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="12"/>
       <c r="B43" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="16" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="17" t="s">
+      <c r="B44" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B44" s="2" t="s">
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="16"/>
+      <c r="B45" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="17"/>
-      <c r="B45" s="2" t="s">
+    <row r="46" spans="1:2">
+      <c r="A46" s="16"/>
+      <c r="B46" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="17"/>
-      <c r="B46" s="2" t="s">
+    <row r="47" spans="1:2">
+      <c r="A47" s="16" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="17" t="s">
+      <c r="B47" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B47" s="2" t="s">
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="16"/>
+      <c r="B48" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="17"/>
-      <c r="B48" s="4" t="s">
+    <row r="49" spans="1:2">
+      <c r="A49" s="16"/>
+      <c r="B49" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="17"/>
-      <c r="B49" s="4" t="s">
+    <row r="50" spans="1:2">
+      <c r="A50" s="16"/>
+      <c r="B50" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="17"/>
-      <c r="B50" s="4" t="s">
+    <row r="51" spans="1:2">
+      <c r="A51" s="16"/>
+      <c r="B51" s="4" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="17"/>
-      <c r="B51" s="4" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B52" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B52" s="4" t="s">
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="16" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="17" t="s">
+      <c r="B53" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B53" s="4" t="s">
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="16"/>
+      <c r="B54" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="17"/>
-      <c r="B54" s="4" t="s">
+    <row r="55" spans="1:2">
+      <c r="A55" s="16"/>
+      <c r="B55" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="17"/>
-      <c r="B55" s="4" t="s">
+    <row r="56" spans="1:2">
+      <c r="A56" s="16"/>
+      <c r="B56" s="4" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="17"/>
-      <c r="B56" s="4" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="4" t="s">
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="16" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="17" t="s">
+      <c r="B58" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B58" s="4" t="s">
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="16"/>
+      <c r="B59" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="16"/>
+      <c r="B60" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="16" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="17"/>
-      <c r="B59" s="4" t="s">
+      <c r="B61" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="16"/>
+      <c r="B62" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="16"/>
+      <c r="B63" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="16"/>
+      <c r="B64" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="16"/>
+      <c r="B65" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="16"/>
+      <c r="B66" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="16"/>
+      <c r="B68" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="16"/>
+      <c r="B69" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="16"/>
+      <c r="B71" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="16"/>
+      <c r="B72" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="16"/>
+      <c r="B73" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="16"/>
+      <c r="B74" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="16"/>
+      <c r="B75" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="16"/>
+      <c r="B76" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="16"/>
+      <c r="B77" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="16"/>
+      <c r="B78" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="16"/>
+      <c r="B79" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="B80" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="17"/>
-      <c r="B60" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="17"/>
-      <c r="B62" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="17"/>
-      <c r="B63" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="17"/>
-      <c r="B64" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="17"/>
-      <c r="B65" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="17"/>
-      <c r="B66" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="17"/>
-      <c r="B68" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="17"/>
-      <c r="B69" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
-      <c r="A71" s="17"/>
-      <c r="B71" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
-      <c r="A72" s="17"/>
-      <c r="B72" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="17"/>
-      <c r="B73" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
-      <c r="A74" s="17"/>
-      <c r="B74" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
-      <c r="A75" s="17"/>
-      <c r="B75" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
-      <c r="A76" s="17"/>
-      <c r="B76" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="A77" s="17"/>
-      <c r="B77" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
-      <c r="A78" s="17"/>
-      <c r="B78" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2">
-      <c r="A79" s="17"/>
-      <c r="B79" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2">
-      <c r="A80" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="B80" s="4" t="s">
+    <row r="81" spans="1:2">
+      <c r="A81" s="16"/>
+      <c r="B81" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="17"/>
-      <c r="B81" s="4" t="s">
+    <row r="82" spans="1:2">
+      <c r="A82" s="16"/>
+      <c r="B82" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="17"/>
-      <c r="B82" s="4" t="s">
+    <row r="83" spans="1:2">
+      <c r="A83" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="16"/>
+      <c r="B84" s="4" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="17"/>
-      <c r="B84" s="4" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1543,39 +1556,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>117</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>120</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>122</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
List methods & comprehension refined
</commit_message>
<xml_diff>
--- a/python_syllabus.xlsx
+++ b/python_syllabus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0893D8F3-681C-4805-852A-D10333F8BD2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EC2B34-82A9-4062-BFE2-8C4B63E10BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -585,15 +585,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -602,18 +614,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -893,7 +893,7 @@
   <dimension ref="A1:E87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -907,14 +907,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="D1" s="11" t="s">
+      <c r="B1" s="15"/>
+      <c r="D1" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="E1" s="11"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
@@ -937,7 +937,7 @@
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="17" t="s">
         <v>102</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -949,7 +949,7 @@
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="14"/>
+      <c r="D4" s="18"/>
       <c r="E4" s="4" t="s">
         <v>108</v>
       </c>
@@ -959,7 +959,7 @@
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="14"/>
+      <c r="D5" s="18"/>
       <c r="E5" s="4" t="s">
         <v>110</v>
       </c>
@@ -969,7 +969,7 @@
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="14"/>
+      <c r="D6" s="18"/>
       <c r="E6" s="4" t="s">
         <v>112</v>
       </c>
@@ -979,7 +979,7 @@
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="14"/>
+      <c r="D7" s="18"/>
       <c r="E7" s="4" t="s">
         <v>113</v>
       </c>
@@ -989,7 +989,7 @@
       <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="15"/>
+      <c r="D8" s="19"/>
       <c r="E8" s="4" t="s">
         <v>109</v>
       </c>
@@ -1157,7 +1157,7 @@
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="13" t="s">
         <v>76</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -1165,7 +1165,7 @@
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="18"/>
+      <c r="A35" s="14"/>
       <c r="B35" s="2" t="s">
         <v>103</v>
       </c>
@@ -1221,7 +1221,7 @@
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="16" t="s">
+      <c r="A44" s="10" t="s">
         <v>39</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -1229,19 +1229,19 @@
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="16"/>
+      <c r="A45" s="10"/>
       <c r="B45" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="16"/>
+      <c r="A46" s="10"/>
       <c r="B46" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="16" t="s">
+      <c r="A47" s="10" t="s">
         <v>43</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -1249,25 +1249,25 @@
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="16"/>
+      <c r="A48" s="10"/>
       <c r="B48" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="16"/>
+      <c r="A49" s="10"/>
       <c r="B49" s="4" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50" s="16"/>
+      <c r="A50" s="10"/>
       <c r="B50" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:2">
-      <c r="A51" s="16"/>
+      <c r="A51" s="10"/>
       <c r="B51" s="4" t="s">
         <v>48</v>
       </c>
@@ -1281,7 +1281,7 @@
       </c>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="16" t="s">
+      <c r="A53" s="10" t="s">
         <v>51</v>
       </c>
       <c r="B53" s="4" t="s">
@@ -1289,19 +1289,19 @@
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="16"/>
+      <c r="A54" s="10"/>
       <c r="B54" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="16"/>
+      <c r="A55" s="10"/>
       <c r="B55" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="16"/>
+      <c r="A56" s="10"/>
       <c r="B56" s="4" t="s">
         <v>55</v>
       </c>
@@ -1315,7 +1315,7 @@
       </c>
     </row>
     <row r="58" spans="1:2">
-      <c r="A58" s="16" t="s">
+      <c r="A58" s="10" t="s">
         <v>58</v>
       </c>
       <c r="B58" s="4" t="s">
@@ -1323,19 +1323,19 @@
       </c>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="16"/>
+      <c r="A59" s="10"/>
       <c r="B59" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="60" spans="1:2">
-      <c r="A60" s="16"/>
+      <c r="A60" s="10"/>
       <c r="B60" s="4" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="61" spans="1:2">
-      <c r="A61" s="16" t="s">
+      <c r="A61" s="10" t="s">
         <v>60</v>
       </c>
       <c r="B61" s="4" t="s">
@@ -1343,37 +1343,37 @@
       </c>
     </row>
     <row r="62" spans="1:2">
-      <c r="A62" s="16"/>
+      <c r="A62" s="10"/>
       <c r="B62" s="4" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="63" spans="1:2">
-      <c r="A63" s="16"/>
+      <c r="A63" s="10"/>
       <c r="B63" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="16"/>
+      <c r="A64" s="10"/>
       <c r="B64" s="4" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="65" spans="1:2">
-      <c r="A65" s="16"/>
+      <c r="A65" s="10"/>
       <c r="B65" s="4" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="66" spans="1:2">
-      <c r="A66" s="16"/>
+      <c r="A66" s="10"/>
       <c r="B66" s="4" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:2">
-      <c r="A67" s="19" t="s">
+      <c r="A67" s="11" t="s">
         <v>85</v>
       </c>
       <c r="B67" s="4" t="s">
@@ -1381,19 +1381,19 @@
       </c>
     </row>
     <row r="68" spans="1:2">
-      <c r="A68" s="16"/>
+      <c r="A68" s="10"/>
       <c r="B68" s="4" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:2">
-      <c r="A69" s="16"/>
+      <c r="A69" s="10"/>
       <c r="B69" s="4" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:2">
-      <c r="A70" s="16" t="s">
+      <c r="A70" s="10" t="s">
         <v>68</v>
       </c>
       <c r="B70" s="4" t="s">
@@ -1401,61 +1401,61 @@
       </c>
     </row>
     <row r="71" spans="1:2">
-      <c r="A71" s="16"/>
+      <c r="A71" s="10"/>
       <c r="B71" s="4" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="16"/>
+      <c r="A72" s="10"/>
       <c r="B72" s="4" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="73" spans="1:2">
-      <c r="A73" s="16"/>
+      <c r="A73" s="10"/>
       <c r="B73" s="4" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="74" spans="1:2">
-      <c r="A74" s="16"/>
+      <c r="A74" s="10"/>
       <c r="B74" s="4" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="75" spans="1:2">
-      <c r="A75" s="16"/>
+      <c r="A75" s="10"/>
       <c r="B75" s="4" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="76" spans="1:2">
-      <c r="A76" s="16"/>
+      <c r="A76" s="10"/>
       <c r="B76" s="4" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="77" spans="1:2">
-      <c r="A77" s="16"/>
+      <c r="A77" s="10"/>
       <c r="B77" s="4" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="78" spans="1:2">
-      <c r="A78" s="16"/>
+      <c r="A78" s="10"/>
       <c r="B78" s="4" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="79" spans="1:2">
-      <c r="A79" s="16"/>
+      <c r="A79" s="10"/>
       <c r="B79" s="4" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="80" spans="1:2">
-      <c r="A80" s="16" t="s">
+      <c r="A80" s="10" t="s">
         <v>104</v>
       </c>
       <c r="B80" s="4" t="s">
@@ -1463,19 +1463,19 @@
       </c>
     </row>
     <row r="81" spans="1:2">
-      <c r="A81" s="16"/>
+      <c r="A81" s="10"/>
       <c r="B81" s="4" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="82" spans="1:2">
-      <c r="A82" s="16"/>
+      <c r="A82" s="10"/>
       <c r="B82" s="4" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="83" spans="1:2">
-      <c r="A83" s="16" t="s">
+      <c r="A83" s="10" t="s">
         <v>83</v>
       </c>
       <c r="B83" s="5" t="s">
@@ -1483,7 +1483,7 @@
       </c>
     </row>
     <row r="84" spans="1:2">
-      <c r="A84" s="16"/>
+      <c r="A84" s="10"/>
       <c r="B84" s="4" t="s">
         <v>100</v>
       </c>
@@ -1514,6 +1514,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="A16:A24"/>
+    <mergeCell ref="D3:D8"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A36:A43"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A47:A51"/>
+    <mergeCell ref="A34:A35"/>
     <mergeCell ref="A80:A82"/>
     <mergeCell ref="A58:A60"/>
     <mergeCell ref="A83:A84"/>
@@ -1521,18 +1533,6 @@
     <mergeCell ref="A61:A66"/>
     <mergeCell ref="A67:A69"/>
     <mergeCell ref="A70:A79"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A36:A43"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A47:A51"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="A3:A10"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="A16:A24"/>
-    <mergeCell ref="D3:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>